<commit_message>
excel read and write done
</commit_message>
<xml_diff>
--- a/TestData.xlsx
+++ b/TestData.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\G992127\Documents\GitHub\ILR_Automation_TestSuite\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{23E3F7E5-7BFF-488D-BEB2-B444F912093E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{82ACC29B-D9A3-4D2E-AC51-C317E2A57EB6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -46,7 +46,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="358" uniqueCount="182">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="322" uniqueCount="183">
   <si>
     <t>Policy No</t>
   </si>
@@ -593,6 +593,9 @@
   <si>
     <t>Passed</t>
   </si>
+  <si>
+    <t>Age</t>
+  </si>
 </sst>
 </file>
 
@@ -803,7 +806,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="5" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="69">
+  <cellXfs count="61">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
@@ -839,9 +842,6 @@
     <xf numFmtId="164" fontId="6" fillId="4" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="5" fillId="7" borderId="0" xfId="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="9" borderId="1" xfId="0" quotePrefix="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
@@ -851,27 +851,6 @@
     </xf>
     <xf numFmtId="0" fontId="8" fillId="10" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="10" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="9" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="9" borderId="1" xfId="0" quotePrefix="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="9" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="22" fontId="0" fillId="9" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="9" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="10" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
@@ -884,50 +863,9 @@
     <xf numFmtId="49" fontId="10" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="22" fontId="0" fillId="9" borderId="1" xfId="0" quotePrefix="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="8" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="8" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="9" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="9" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="9" borderId="3" xfId="0" quotePrefix="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="9" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="9" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="9" borderId="1" xfId="0" quotePrefix="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="49" fontId="1" fillId="8" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="49" fontId="2" fillId="9" borderId="1" xfId="0" quotePrefix="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -942,13 +880,54 @@
     <xf numFmtId="49" fontId="2" fillId="9" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="49" fontId="12" fillId="9" borderId="1" xfId="0" quotePrefix="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
     <xf numFmtId="49" fontId="0" fillId="9" borderId="1" xfId="0" quotePrefix="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" quotePrefix="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="1" fontId="6" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="49" fontId="1" fillId="8" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="1" xfId="0" quotePrefix="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="9" borderId="3" xfId="0" quotePrefix="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="9" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="9" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="9" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="2" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="9" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="9" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="12" fillId="9" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="12" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="9" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
   </cellXfs>
@@ -970,6 +949,7 @@
         <family val="2"/>
         <scheme val="minor"/>
       </font>
+      <numFmt numFmtId="30" formatCode="@"/>
       <fill>
         <patternFill>
           <fgColor indexed="64"/>
@@ -977,7 +957,7 @@
         </patternFill>
       </fill>
       <alignment horizontal="general" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-      <border diagonalUp="0" diagonalDown="0">
+      <border diagonalUp="0" diagonalDown="0" outline="0">
         <left style="thin">
           <color indexed="64"/>
         </left>
@@ -988,12 +968,6 @@
         <bottom style="thin">
           <color indexed="64"/>
         </bottom>
-        <vertical style="thin">
-          <color indexed="64"/>
-        </vertical>
-        <horizontal style="thin">
-          <color indexed="64"/>
-        </horizontal>
       </border>
     </dxf>
     <dxf>
@@ -1021,7 +995,7 @@
         </patternFill>
       </fill>
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-      <border diagonalUp="0" diagonalDown="0">
+      <border diagonalUp="0" diagonalDown="0" outline="0">
         <left style="thin">
           <color indexed="64"/>
         </left>
@@ -1034,8 +1008,6 @@
         <bottom style="thin">
           <color indexed="64"/>
         </bottom>
-        <vertical/>
-        <horizontal/>
       </border>
     </dxf>
     <dxf>
@@ -1051,6 +1023,7 @@
         <family val="2"/>
         <scheme val="minor"/>
       </font>
+      <numFmt numFmtId="30" formatCode="@"/>
       <fill>
         <patternFill>
           <fgColor indexed="64"/>
@@ -1074,6 +1047,7 @@
       </border>
     </dxf>
     <dxf>
+      <numFmt numFmtId="30" formatCode="@"/>
       <fill>
         <patternFill patternType="solid">
           <fgColor indexed="64"/>
@@ -1108,6 +1082,7 @@
         <family val="2"/>
         <scheme val="minor"/>
       </font>
+      <numFmt numFmtId="30" formatCode="@"/>
       <alignment horizontal="left" vertical="top" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
       <border diagonalUp="0" diagonalDown="0" outline="0">
         <left style="thin">
@@ -1136,8 +1111,9 @@
         <family val="2"/>
         <scheme val="minor"/>
       </font>
+      <numFmt numFmtId="30" formatCode="@"/>
       <alignment horizontal="left" vertical="top" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-      <border diagonalUp="0" diagonalDown="0">
+      <border diagonalUp="0" diagonalDown="0" outline="0">
         <left style="thin">
           <color indexed="64"/>
         </left>
@@ -1150,12 +1126,6 @@
         <bottom style="thin">
           <color indexed="64"/>
         </bottom>
-        <vertical style="thin">
-          <color indexed="64"/>
-        </vertical>
-        <horizontal style="thin">
-          <color indexed="64"/>
-        </horizontal>
       </border>
     </dxf>
     <dxf>
@@ -1170,8 +1140,9 @@
         <family val="2"/>
         <scheme val="minor"/>
       </font>
+      <numFmt numFmtId="30" formatCode="@"/>
       <alignment horizontal="left" vertical="top" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-      <border diagonalUp="0" diagonalDown="0">
+      <border diagonalUp="0" diagonalDown="0" outline="0">
         <left style="thin">
           <color indexed="64"/>
         </left>
@@ -1184,12 +1155,6 @@
         <bottom style="thin">
           <color indexed="64"/>
         </bottom>
-        <vertical style="thin">
-          <color indexed="64"/>
-        </vertical>
-        <horizontal style="thin">
-          <color indexed="64"/>
-        </horizontal>
       </border>
     </dxf>
     <dxf>
@@ -1204,8 +1169,9 @@
         <family val="2"/>
         <scheme val="minor"/>
       </font>
+      <numFmt numFmtId="30" formatCode="@"/>
       <alignment horizontal="left" vertical="top" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-      <border diagonalUp="0" diagonalDown="0">
+      <border diagonalUp="0" diagonalDown="0" outline="0">
         <left style="thin">
           <color indexed="64"/>
         </left>
@@ -1218,12 +1184,6 @@
         <bottom style="thin">
           <color indexed="64"/>
         </bottom>
-        <vertical style="thin">
-          <color indexed="64"/>
-        </vertical>
-        <horizontal style="thin">
-          <color indexed="64"/>
-        </horizontal>
       </border>
     </dxf>
     <dxf>
@@ -1238,8 +1198,9 @@
         <family val="2"/>
         <scheme val="minor"/>
       </font>
+      <numFmt numFmtId="30" formatCode="@"/>
       <alignment horizontal="left" vertical="top" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-      <border diagonalUp="0" diagonalDown="0">
+      <border diagonalUp="0" diagonalDown="0" outline="0">
         <left style="thin">
           <color indexed="64"/>
         </left>
@@ -1252,12 +1213,6 @@
         <bottom style="thin">
           <color indexed="64"/>
         </bottom>
-        <vertical style="thin">
-          <color indexed="64"/>
-        </vertical>
-        <horizontal style="thin">
-          <color indexed="64"/>
-        </horizontal>
       </border>
     </dxf>
     <dxf>
@@ -1272,8 +1227,9 @@
         <family val="2"/>
         <scheme val="minor"/>
       </font>
+      <numFmt numFmtId="30" formatCode="@"/>
       <alignment horizontal="left" vertical="top" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-      <border diagonalUp="0" diagonalDown="0">
+      <border diagonalUp="0" diagonalDown="0" outline="0">
         <left/>
         <right style="thin">
           <color indexed="64"/>
@@ -1284,12 +1240,6 @@
         <bottom style="thin">
           <color indexed="64"/>
         </bottom>
-        <vertical style="thin">
-          <color indexed="64"/>
-        </vertical>
-        <horizontal style="thin">
-          <color indexed="64"/>
-        </horizontal>
       </border>
     </dxf>
     <dxf>
@@ -1316,6 +1266,7 @@
       </border>
     </dxf>
     <dxf>
+      <numFmt numFmtId="30" formatCode="@"/>
       <alignment horizontal="general" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
@@ -1342,13 +1293,14 @@
         <family val="2"/>
         <scheme val="minor"/>
       </font>
+      <numFmt numFmtId="30" formatCode="@"/>
       <fill>
         <patternFill patternType="solid">
           <fgColor indexed="64"/>
           <bgColor theme="9" tint="-0.249977111117893"/>
         </patternFill>
       </fill>
-      <border diagonalUp="0" diagonalDown="0">
+      <border diagonalUp="0" diagonalDown="0" outline="0">
         <left style="thin">
           <color indexed="64"/>
         </left>
@@ -1357,12 +1309,6 @@
         </right>
         <top/>
         <bottom/>
-        <vertical style="thin">
-          <color indexed="64"/>
-        </vertical>
-        <horizontal style="thin">
-          <color indexed="64"/>
-        </horizontal>
       </border>
     </dxf>
   </dxfs>
@@ -1384,8 +1330,8 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{609B3FE1-602A-411C-91B1-C1CE8676CFCE}" name="Table1" displayName="Table1" ref="A1:J14" totalsRowShown="0" headerRowDxfId="14" dataDxfId="12" headerRowBorderDxfId="13" tableBorderDxfId="11" totalsRowBorderDxfId="10">
-  <autoFilter ref="A1:J14" xr:uid="{609B3FE1-602A-411C-91B1-C1CE8676CFCE}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{609B3FE1-602A-411C-91B1-C1CE8676CFCE}" name="Table1" displayName="Table1" ref="A1:J18" totalsRowShown="0" headerRowDxfId="14" dataDxfId="12" headerRowBorderDxfId="13" tableBorderDxfId="11" totalsRowBorderDxfId="10">
+  <autoFilter ref="A1:J18" xr:uid="{609B3FE1-602A-411C-91B1-C1CE8676CFCE}"/>
   <tableColumns count="10">
     <tableColumn id="1" xr3:uid="{F815EF09-5A8D-41CD-9C8D-1F1F859054C1}" name="Policy No" dataDxfId="9"/>
     <tableColumn id="2" xr3:uid="{A75649DE-6DED-4E66-9436-0C7BC08EC505}" name="Function" dataDxfId="8"/>
@@ -1701,29 +1647,29 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{122D3D24-972A-41AA-875A-C35A49A85BBB}">
   <dimension ref="A1:J20"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="C21" sqref="C21"/>
+    <sheetView tabSelected="1" topLeftCell="B1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="H2" sqref="H2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="25.6328125" customWidth="1"/>
-    <col min="2" max="2" width="35.1796875" customWidth="1"/>
-    <col min="3" max="3" width="43.36328125" style="4" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="39.6328125" style="4" customWidth="1"/>
-    <col min="5" max="5" width="16.36328125" customWidth="1"/>
-    <col min="6" max="6" width="25.1796875" customWidth="1"/>
-    <col min="7" max="7" width="17.81640625" customWidth="1"/>
-    <col min="8" max="8" width="16.1796875" customWidth="1"/>
-    <col min="9" max="9" width="34.81640625" style="8" customWidth="1"/>
-    <col min="10" max="10" width="24.81640625" customWidth="1"/>
+    <col min="1" max="1" width="25.6328125" customWidth="1" collapsed="1"/>
+    <col min="2" max="2" width="35.1796875" customWidth="1" collapsed="1"/>
+    <col min="3" max="3" width="43.36328125" style="4" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="4" max="4" width="39.6328125" style="4" customWidth="1" collapsed="1"/>
+    <col min="5" max="5" width="16.36328125" customWidth="1" collapsed="1"/>
+    <col min="6" max="6" width="25.1796875" customWidth="1" collapsed="1"/>
+    <col min="7" max="7" width="17.81640625" customWidth="1" collapsed="1"/>
+    <col min="8" max="8" width="16.1796875" customWidth="1" collapsed="1"/>
+    <col min="9" max="9" width="34.81640625" style="8" customWidth="1" collapsed="1"/>
+    <col min="10" max="10" width="24.81640625" customWidth="1" collapsed="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:10" s="1" customFormat="1" ht="18.5" x14ac:dyDescent="0.45">
-      <c r="A1" s="45" t="s">
+      <c r="A1" s="38" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="45" t="s">
+      <c r="B1" s="38" t="s">
         <v>1</v>
       </c>
       <c r="C1" s="46" t="s">
@@ -1732,247 +1678,277 @@
       <c r="D1" s="46" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="45" t="s">
+      <c r="E1" s="38" t="s">
         <v>6</v>
       </c>
-      <c r="F1" s="45" t="s">
+      <c r="F1" s="38" t="s">
         <v>4</v>
       </c>
-      <c r="G1" s="45" t="s">
+      <c r="G1" s="38" t="s">
         <v>5</v>
       </c>
-      <c r="H1" s="45" t="s">
+      <c r="H1" s="38" t="s">
         <v>7</v>
       </c>
-      <c r="I1" s="61" t="s">
+      <c r="I1" s="38" t="s">
         <v>178</v>
       </c>
-      <c r="J1" s="45" t="s">
+      <c r="J1" s="38" t="s">
         <v>8</v>
       </c>
     </row>
     <row r="2" spans="1:10" ht="37.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A2" s="38" t="s">
+      <c r="A2" s="47" t="s">
         <v>77</v>
       </c>
-      <c r="B2" s="38" t="s">
+      <c r="B2" s="47" t="s">
         <v>76</v>
       </c>
-      <c r="C2" s="38"/>
-      <c r="D2" s="38"/>
-      <c r="E2" s="68" t="s">
+      <c r="C2" s="47"/>
+      <c r="D2" s="47"/>
+      <c r="E2" s="48" t="s">
         <v>179</v>
       </c>
-      <c r="F2" s="38"/>
+      <c r="F2" s="47" t="s">
+        <v>181</v>
+      </c>
       <c r="G2" s="49"/>
-      <c r="H2" s="34" t="s">
+      <c r="H2" s="39"/>
+      <c r="I2" s="39"/>
+      <c r="J2" s="43"/>
+    </row>
+    <row r="3" spans="1:10" ht="29" x14ac:dyDescent="0.35">
+      <c r="A3" s="50" t="s">
+        <v>77</v>
+      </c>
+      <c r="B3" s="47" t="s">
+        <v>180</v>
+      </c>
+      <c r="C3" s="47"/>
+      <c r="D3" s="47"/>
+      <c r="E3" s="48" t="s">
+        <v>179</v>
+      </c>
+      <c r="F3" s="47" t="s">
         <v>181</v>
       </c>
-      <c r="I2" s="62"/>
-      <c r="J2" s="27"/>
-    </row>
-    <row r="3" spans="1:10" ht="29" x14ac:dyDescent="0.35">
-      <c r="A3" s="54" t="s">
-        <v>77</v>
-      </c>
-      <c r="B3" s="38" t="s">
-        <v>180</v>
-      </c>
-      <c r="C3" s="38"/>
-      <c r="D3" s="38"/>
-      <c r="E3" s="68" t="s">
-        <v>179</v>
-      </c>
-      <c r="F3" s="38"/>
       <c r="G3" s="49"/>
-      <c r="H3" s="34" t="s">
+      <c r="H3" s="39"/>
+      <c r="I3" s="40"/>
+      <c r="J3" s="51"/>
+    </row>
+    <row r="4" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="A4" s="50"/>
+      <c r="B4" s="47"/>
+      <c r="C4" s="47"/>
+      <c r="D4" s="47"/>
+      <c r="E4" s="47"/>
+      <c r="F4" s="47" t="s">
         <v>181</v>
       </c>
-      <c r="I3" s="63"/>
-      <c r="J3" s="55"/>
-    </row>
-    <row r="4" spans="1:10" x14ac:dyDescent="0.35">
-      <c r="A4" s="54"/>
-      <c r="B4" s="38"/>
-      <c r="C4" s="38"/>
-      <c r="D4" s="38"/>
-      <c r="E4" s="38"/>
-      <c r="F4" s="38"/>
       <c r="G4" s="49"/>
-      <c r="H4" s="35"/>
-      <c r="I4" s="64"/>
-      <c r="J4" s="56"/>
+      <c r="H4" s="42"/>
+      <c r="I4" s="41"/>
+      <c r="J4" s="52"/>
     </row>
     <row r="5" spans="1:10" x14ac:dyDescent="0.35">
-      <c r="A5" s="38"/>
-      <c r="B5" s="38"/>
-      <c r="C5" s="38"/>
-      <c r="D5" s="38"/>
-      <c r="E5" s="38"/>
-      <c r="F5" s="38"/>
+      <c r="A5" s="47"/>
+      <c r="B5" s="47"/>
+      <c r="C5" s="47"/>
+      <c r="D5" s="47"/>
+      <c r="E5" s="47"/>
+      <c r="F5" s="47" t="s">
+        <v>181</v>
+      </c>
       <c r="G5" s="49"/>
-      <c r="H5" s="34"/>
-      <c r="I5" s="62"/>
-      <c r="J5" s="27"/>
+      <c r="H5" s="39"/>
+      <c r="I5" s="39"/>
+      <c r="J5" s="43"/>
     </row>
     <row r="6" spans="1:10" x14ac:dyDescent="0.35">
-      <c r="A6" s="38"/>
-      <c r="B6" s="38"/>
-      <c r="C6" s="38"/>
-      <c r="D6" s="38"/>
-      <c r="E6" s="38"/>
-      <c r="F6" s="38"/>
+      <c r="A6" s="47"/>
+      <c r="B6" s="47"/>
+      <c r="C6" s="47"/>
+      <c r="D6" s="47"/>
+      <c r="E6" s="47"/>
+      <c r="F6" s="47" t="s">
+        <v>181</v>
+      </c>
       <c r="G6" s="49"/>
-      <c r="H6" s="34"/>
-      <c r="I6" s="62"/>
-      <c r="J6" s="27"/>
+      <c r="H6" s="39"/>
+      <c r="I6" s="39"/>
+      <c r="J6" s="43"/>
     </row>
     <row r="7" spans="1:10" x14ac:dyDescent="0.35">
-      <c r="A7" s="38"/>
-      <c r="B7" s="38"/>
-      <c r="C7" s="38"/>
-      <c r="D7" s="38"/>
-      <c r="E7" s="38"/>
-      <c r="F7" s="38"/>
+      <c r="A7" s="47"/>
+      <c r="B7" s="47"/>
+      <c r="C7" s="47"/>
+      <c r="D7" s="47"/>
+      <c r="E7" s="47"/>
+      <c r="F7" s="47" t="s">
+        <v>181</v>
+      </c>
       <c r="G7" s="49"/>
-      <c r="H7" s="35"/>
-      <c r="I7" s="65"/>
-      <c r="J7" s="36"/>
+      <c r="H7" s="42"/>
+      <c r="I7" s="42"/>
+      <c r="J7" s="53"/>
     </row>
     <row r="8" spans="1:10" x14ac:dyDescent="0.35">
-      <c r="A8" s="38"/>
-      <c r="B8" s="38"/>
-      <c r="C8" s="38"/>
-      <c r="D8" s="38"/>
-      <c r="E8" s="38"/>
-      <c r="F8" s="38"/>
+      <c r="A8" s="47"/>
+      <c r="B8" s="47"/>
+      <c r="C8" s="47"/>
+      <c r="D8" s="47"/>
+      <c r="E8" s="47"/>
+      <c r="F8" s="47" t="s">
+        <v>181</v>
+      </c>
       <c r="G8" s="49"/>
-      <c r="H8" s="34"/>
-      <c r="I8" s="62"/>
-      <c r="J8" s="44"/>
+      <c r="H8" s="39"/>
+      <c r="I8" s="39"/>
+      <c r="J8" s="43"/>
     </row>
     <row r="9" spans="1:10" x14ac:dyDescent="0.35">
-      <c r="A9" s="38"/>
-      <c r="B9" s="38"/>
-      <c r="C9" s="38"/>
-      <c r="D9" s="38"/>
-      <c r="E9" s="38"/>
-      <c r="F9" s="38"/>
+      <c r="A9" s="47"/>
+      <c r="B9" s="47"/>
+      <c r="C9" s="47"/>
+      <c r="D9" s="47"/>
+      <c r="E9" s="47"/>
+      <c r="F9" s="47" t="s">
+        <v>181</v>
+      </c>
       <c r="G9" s="49"/>
-      <c r="H9" s="34"/>
-      <c r="I9" s="62"/>
-      <c r="J9" s="27"/>
+      <c r="H9" s="39"/>
+      <c r="I9" s="39"/>
+      <c r="J9" s="43"/>
     </row>
     <row r="10" spans="1:10" x14ac:dyDescent="0.35">
-      <c r="A10" s="38"/>
-      <c r="B10" s="38"/>
-      <c r="C10" s="47"/>
-      <c r="D10" s="38"/>
-      <c r="E10" s="38"/>
-      <c r="F10" s="38"/>
+      <c r="A10" s="47"/>
+      <c r="B10" s="47"/>
+      <c r="C10" s="54"/>
+      <c r="D10" s="47"/>
+      <c r="E10" s="47"/>
+      <c r="F10" s="47" t="s">
+        <v>181</v>
+      </c>
       <c r="G10" s="49"/>
-      <c r="H10" s="35"/>
-      <c r="I10" s="65"/>
-      <c r="J10" s="37"/>
+      <c r="H10" s="42"/>
+      <c r="I10" s="42"/>
+      <c r="J10" s="53"/>
     </row>
     <row r="11" spans="1:10" x14ac:dyDescent="0.35">
-      <c r="A11" s="39"/>
-      <c r="B11" s="38"/>
-      <c r="C11" s="38"/>
-      <c r="D11" s="38"/>
-      <c r="E11" s="38"/>
-      <c r="F11" s="38"/>
+      <c r="A11" s="55"/>
+      <c r="B11" s="47"/>
+      <c r="C11" s="47"/>
+      <c r="D11" s="47"/>
+      <c r="E11" s="47"/>
+      <c r="F11" s="47" t="s">
+        <v>181</v>
+      </c>
       <c r="G11" s="49"/>
-      <c r="H11" s="35"/>
-      <c r="I11" s="65"/>
-      <c r="J11" s="37"/>
+      <c r="H11" s="42"/>
+      <c r="I11" s="42"/>
+      <c r="J11" s="53"/>
     </row>
     <row r="12" spans="1:10" x14ac:dyDescent="0.35">
-      <c r="A12" s="38"/>
-      <c r="B12" s="38"/>
-      <c r="C12" s="38"/>
-      <c r="D12" s="38"/>
-      <c r="E12" s="38"/>
-      <c r="F12" s="38"/>
+      <c r="A12" s="47"/>
+      <c r="B12" s="47"/>
+      <c r="C12" s="47"/>
+      <c r="D12" s="47"/>
+      <c r="E12" s="47"/>
+      <c r="F12" s="47" t="s">
+        <v>181</v>
+      </c>
       <c r="G12" s="49"/>
-      <c r="H12" s="35"/>
-      <c r="I12" s="65"/>
-      <c r="J12" s="37"/>
+      <c r="H12" s="42"/>
+      <c r="I12" s="42"/>
+      <c r="J12" s="53"/>
     </row>
     <row r="13" spans="1:10" x14ac:dyDescent="0.35">
-      <c r="A13" s="38"/>
-      <c r="B13" s="38"/>
-      <c r="C13" s="38"/>
-      <c r="D13" s="38"/>
-      <c r="E13" s="38"/>
-      <c r="F13" s="38"/>
+      <c r="A13" s="47"/>
+      <c r="B13" s="47"/>
+      <c r="C13" s="47"/>
+      <c r="D13" s="47"/>
+      <c r="E13" s="47"/>
+      <c r="F13" s="47" t="s">
+        <v>181</v>
+      </c>
       <c r="G13" s="49"/>
-      <c r="H13" s="35"/>
-      <c r="I13" s="65"/>
-      <c r="J13" s="37"/>
+      <c r="H13" s="42"/>
+      <c r="I13" s="42"/>
+      <c r="J13" s="53"/>
     </row>
     <row r="14" spans="1:10" x14ac:dyDescent="0.35">
-      <c r="A14" s="38"/>
-      <c r="B14" s="38"/>
-      <c r="C14" s="38"/>
-      <c r="D14" s="38"/>
-      <c r="E14" s="38"/>
-      <c r="F14" s="38"/>
-      <c r="G14" s="33"/>
-      <c r="H14" s="35"/>
-      <c r="I14" s="65"/>
-      <c r="J14" s="37"/>
+      <c r="A14" s="47"/>
+      <c r="B14" s="47"/>
+      <c r="C14" s="47"/>
+      <c r="D14" s="47"/>
+      <c r="E14" s="47"/>
+      <c r="F14" s="47" t="s">
+        <v>181</v>
+      </c>
+      <c r="G14" s="56"/>
+      <c r="H14" s="42"/>
+      <c r="I14" s="42"/>
+      <c r="J14" s="53"/>
     </row>
     <row r="15" spans="1:10" x14ac:dyDescent="0.35">
-      <c r="A15" s="38"/>
-      <c r="B15" s="38"/>
-      <c r="C15" s="38"/>
-      <c r="D15" s="38"/>
-      <c r="E15" s="38"/>
-      <c r="F15" s="38"/>
+      <c r="A15" s="50"/>
+      <c r="B15" s="47"/>
+      <c r="C15" s="47"/>
+      <c r="D15" s="47"/>
+      <c r="E15" s="47"/>
+      <c r="F15" s="47" t="s">
+        <v>181</v>
+      </c>
       <c r="G15" s="49"/>
-      <c r="H15" s="34"/>
-      <c r="I15" s="62"/>
-      <c r="J15" s="27"/>
+      <c r="H15" s="39"/>
+      <c r="I15" s="39"/>
+      <c r="J15" s="51"/>
     </row>
     <row r="16" spans="1:10" x14ac:dyDescent="0.35">
-      <c r="A16" s="50"/>
-      <c r="B16" s="50"/>
-      <c r="C16" s="50"/>
-      <c r="D16" s="50"/>
-      <c r="E16" s="57"/>
-      <c r="F16" s="58"/>
+      <c r="A16" s="60"/>
+      <c r="B16" s="57"/>
+      <c r="C16" s="57"/>
+      <c r="D16" s="57"/>
+      <c r="E16" s="58"/>
+      <c r="F16" s="47" t="s">
+        <v>181</v>
+      </c>
       <c r="G16" s="59"/>
-      <c r="H16" s="60"/>
-      <c r="I16" s="66"/>
-      <c r="J16" s="60"/>
+      <c r="H16" s="39"/>
+      <c r="I16" s="39"/>
+      <c r="J16" s="51"/>
     </row>
     <row r="17" spans="1:10" x14ac:dyDescent="0.35">
-      <c r="A17" s="38"/>
-      <c r="B17" s="26"/>
-      <c r="C17" s="26"/>
-      <c r="D17" s="48"/>
-      <c r="E17" s="38"/>
-      <c r="F17" s="26"/>
-      <c r="G17" s="26"/>
-      <c r="H17" s="27"/>
-      <c r="I17" s="67"/>
-      <c r="J17" s="27"/>
+      <c r="A17" s="50"/>
+      <c r="B17" s="47"/>
+      <c r="C17" s="47"/>
+      <c r="D17" s="47"/>
+      <c r="E17" s="47"/>
+      <c r="F17" s="47" t="s">
+        <v>181</v>
+      </c>
+      <c r="G17" s="49"/>
+      <c r="H17" s="39"/>
+      <c r="I17" s="39"/>
+      <c r="J17" s="51"/>
     </row>
     <row r="18" spans="1:10" x14ac:dyDescent="0.35">
-      <c r="A18" s="50"/>
-      <c r="B18" s="51"/>
-      <c r="C18" s="51"/>
-      <c r="D18" s="33"/>
-      <c r="E18" s="50"/>
-      <c r="F18" s="51"/>
-      <c r="G18" s="51"/>
-      <c r="H18" s="27"/>
-      <c r="I18" s="67"/>
-      <c r="J18" s="27"/>
+      <c r="A18" s="60"/>
+      <c r="B18" s="57"/>
+      <c r="C18" s="57"/>
+      <c r="D18" s="57"/>
+      <c r="E18" s="57"/>
+      <c r="F18" s="47" t="s">
+        <v>181</v>
+      </c>
+      <c r="G18" s="49"/>
+      <c r="H18" s="39"/>
+      <c r="I18" s="39"/>
+      <c r="J18" s="51"/>
     </row>
     <row r="20" spans="1:10" x14ac:dyDescent="0.35">
-      <c r="J20" s="52"/>
+      <c r="J20" s="36"/>
     </row>
   </sheetData>
   <phoneticPr fontId="3" type="noConversion"/>
@@ -1994,64 +1970,64 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="7" max="7" width="12.08984375" customWidth="1"/>
+    <col min="7" max="7" width="12.08984375" customWidth="1" collapsed="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:9" x14ac:dyDescent="0.35">
-      <c r="A1" s="40" t="s">
+      <c r="A1" s="32" t="s">
         <v>13</v>
       </c>
-      <c r="B1" s="40" t="s">
+      <c r="B1" s="32" t="s">
         <v>150</v>
       </c>
-      <c r="C1" s="40" t="s">
+      <c r="C1" s="32" t="s">
         <v>11</v>
       </c>
-      <c r="D1" s="40" t="s">
+      <c r="D1" s="32" t="s">
         <v>151</v>
       </c>
-      <c r="E1" s="40" t="s">
+      <c r="E1" s="32" t="s">
         <v>14</v>
       </c>
-      <c r="F1" s="40" t="s">
+      <c r="F1" s="32" t="s">
         <v>15</v>
       </c>
-      <c r="G1" s="40" t="s">
+      <c r="G1" s="32" t="s">
         <v>152</v>
       </c>
-      <c r="H1" s="40" t="s">
+      <c r="H1" s="32" t="s">
         <v>153</v>
       </c>
-      <c r="I1" s="40" t="s">
+      <c r="I1" s="32" t="s">
         <v>154</v>
       </c>
     </row>
     <row r="2" spans="1:9" x14ac:dyDescent="0.35">
-      <c r="A2" s="40" t="s">
+      <c r="A2" s="32" t="s">
         <v>18</v>
       </c>
-      <c r="B2" s="40" t="s">
+      <c r="B2" s="32" t="s">
         <v>164</v>
       </c>
-      <c r="C2" s="40" t="s">
+      <c r="C2" s="32" t="s">
         <v>155</v>
       </c>
-      <c r="D2" s="40" t="s">
+      <c r="D2" s="32" t="s">
         <v>165</v>
       </c>
-      <c r="E2" s="43" t="s">
+      <c r="E2" s="35" t="s">
         <v>167</v>
       </c>
-      <c r="F2" s="40" t="s">
+      <c r="F2" s="32" t="s">
         <v>17</v>
       </c>
-      <c r="G2" s="42" t="s">
+      <c r="G2" s="34" t="s">
         <v>175</v>
       </c>
-      <c r="H2" s="40" t="s">
+      <c r="H2" s="32" t="s">
         <v>156</v>
       </c>
-      <c r="I2" s="43" t="s">
+      <c r="I2" s="35" t="s">
         <v>166</v>
       </c>
     </row>
@@ -2070,31 +2046,31 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="9.6328125" customWidth="1"/>
-    <col min="2" max="2" width="11.1796875" customWidth="1"/>
-    <col min="3" max="3" width="14.1796875" customWidth="1"/>
-    <col min="4" max="4" width="29.36328125" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="21.26953125" customWidth="1"/>
-    <col min="6" max="6" width="20.90625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="9.6328125" customWidth="1" collapsed="1"/>
+    <col min="2" max="2" width="11.1796875" customWidth="1" collapsed="1"/>
+    <col min="3" max="3" width="14.1796875" customWidth="1" collapsed="1"/>
+    <col min="4" max="4" width="29.36328125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="5" max="5" width="21.26953125" customWidth="1" collapsed="1"/>
+    <col min="6" max="6" width="20.90625" bestFit="1" customWidth="1" collapsed="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:6" ht="15.5" x14ac:dyDescent="0.35">
-      <c r="A1" s="29" t="s">
+      <c r="A1" s="28" t="s">
         <v>13</v>
       </c>
-      <c r="B1" s="29" t="s">
+      <c r="B1" s="28" t="s">
         <v>11</v>
       </c>
-      <c r="C1" s="30" t="s">
+      <c r="C1" s="29" t="s">
         <v>80</v>
       </c>
-      <c r="D1" s="30" t="s">
+      <c r="D1" s="29" t="s">
         <v>79</v>
       </c>
-      <c r="E1" s="31" t="s">
+      <c r="E1" s="30" t="s">
         <v>78</v>
       </c>
-      <c r="F1" s="32" t="s">
+      <c r="F1" s="31" t="s">
         <v>81</v>
       </c>
     </row>
@@ -2105,7 +2081,7 @@
       <c r="B2" s="26" t="s">
         <v>106</v>
       </c>
-      <c r="C2" s="28" t="s">
+      <c r="C2" s="27" t="s">
         <v>112</v>
       </c>
       <c r="D2" s="26" t="s">
@@ -2174,7 +2150,7 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="9" max="9" width="9.36328125" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="9.36328125" bestFit="1" customWidth="1" collapsed="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:42" x14ac:dyDescent="0.35">
@@ -9030,11 +9006,11 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="79.26953125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="34.08984375" customWidth="1"/>
-    <col min="3" max="3" width="27.1796875" customWidth="1"/>
-    <col min="4" max="4" width="34.54296875" customWidth="1"/>
-    <col min="5" max="5" width="29.36328125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="79.26953125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="2" max="2" width="34.08984375" customWidth="1" collapsed="1"/>
+    <col min="3" max="3" width="27.1796875" customWidth="1" collapsed="1"/>
+    <col min="4" max="4" width="34.54296875" customWidth="1" collapsed="1"/>
+    <col min="5" max="5" width="29.36328125" bestFit="1" customWidth="1" collapsed="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:6" x14ac:dyDescent="0.35">
@@ -9310,7 +9286,7 @@
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F58BF590-A1C4-40D9-A7C3-D99681DD5C9A}">
-  <dimension ref="A1:H3"/>
+  <dimension ref="A1:I3"/>
   <sheetViews>
     <sheetView topLeftCell="AE1" workbookViewId="0">
       <selection activeCell="E4" sqref="E4"/>
@@ -9318,14 +9294,14 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="2" max="2" width="10.81640625" customWidth="1"/>
-    <col min="3" max="3" width="16.26953125" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="15.6328125" style="6" customWidth="1"/>
-    <col min="5" max="5" width="16.36328125" customWidth="1"/>
-    <col min="6" max="6" width="19.08984375" style="8" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="16.08984375" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="14.453125" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="11.81640625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="10.81640625" customWidth="1" collapsed="1"/>
+    <col min="3" max="3" width="16.26953125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="4" max="4" width="15.6328125" style="6" customWidth="1" collapsed="1"/>
+    <col min="5" max="5" width="16.36328125" customWidth="1" collapsed="1"/>
+    <col min="6" max="6" width="19.08984375" style="8" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="7" max="7" width="16.08984375" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="8" max="8" width="14.453125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="9" max="9" width="11.81640625" bestFit="1" customWidth="1" collapsed="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:8" s="1" customFormat="1" ht="18.5" x14ac:dyDescent="0.45">
@@ -9386,23 +9362,23 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="13" max="13" width="17.36328125" customWidth="1"/>
-    <col min="14" max="14" width="16.54296875" customWidth="1"/>
+    <col min="13" max="13" width="17.36328125" customWidth="1" collapsed="1"/>
+    <col min="14" max="14" width="16.54296875" customWidth="1" collapsed="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="13:14" x14ac:dyDescent="0.35">
-      <c r="M1" s="32" t="s">
+      <c r="M1" s="31" t="s">
         <v>176</v>
       </c>
-      <c r="N1" s="32" t="s">
+      <c r="N1" s="31" t="s">
         <v>177</v>
       </c>
     </row>
     <row r="2" spans="13:14" x14ac:dyDescent="0.35">
-      <c r="M2" s="53">
+      <c r="M2" s="37">
         <v>87678765</v>
       </c>
-      <c r="N2" s="53">
+      <c r="N2" s="37">
         <v>87688765</v>
       </c>
     </row>
@@ -9414,22 +9390,23 @@
 
 <file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3F5E7B35-3B13-4283-A904-8C8CA7625FAB}">
-  <dimension ref="A1:AY88"/>
+  <dimension ref="A1:AY87"/>
   <sheetViews>
-    <sheetView topLeftCell="Y1" workbookViewId="0">
-      <selection activeCell="G12" sqref="G12"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="E8" sqref="E8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="3" max="3" width="10.90625" customWidth="1"/>
-    <col min="4" max="4" width="9.1796875" customWidth="1"/>
-    <col min="15" max="15" width="12.81640625" customWidth="1"/>
+    <col min="1" max="1" width="8.7265625" style="45" collapsed="1"/>
+    <col min="3" max="3" width="10.90625" customWidth="1" collapsed="1"/>
+    <col min="4" max="4" width="9.1796875" customWidth="1" collapsed="1"/>
+    <col min="15" max="15" width="12.81640625" customWidth="1" collapsed="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:51" x14ac:dyDescent="0.35">
-      <c r="A1" s="21" t="s">
-        <v>21</v>
+      <c r="A1" s="44" t="s">
+        <v>182</v>
       </c>
       <c r="B1" s="21" t="s">
         <v>22</v>
@@ -9583,163 +9560,47 @@
       </c>
     </row>
     <row r="2" spans="1:51" x14ac:dyDescent="0.35">
-      <c r="A2" s="21" t="s">
-        <v>62</v>
-      </c>
-      <c r="B2" s="21" t="s">
-        <v>62</v>
-      </c>
-      <c r="C2" s="21" t="s">
-        <v>62</v>
-      </c>
-      <c r="D2" s="21" t="s">
-        <v>62</v>
-      </c>
-      <c r="E2" s="21" t="s">
-        <v>62</v>
-      </c>
-      <c r="F2" s="21" t="s">
-        <v>62</v>
-      </c>
-      <c r="G2" s="21" t="s">
-        <v>62</v>
-      </c>
-      <c r="H2" s="21" t="s">
-        <v>62</v>
-      </c>
-      <c r="I2" s="21" t="s">
-        <v>62</v>
-      </c>
-      <c r="J2" s="21" t="s">
-        <v>62</v>
-      </c>
-      <c r="K2" s="21" t="s">
-        <v>62</v>
-      </c>
-      <c r="L2" s="21" t="s">
-        <v>62</v>
-      </c>
-      <c r="M2" s="21" t="s">
-        <v>62</v>
-      </c>
-      <c r="N2" s="22" t="s">
-        <v>62</v>
-      </c>
-      <c r="O2" s="21" t="s">
-        <v>62</v>
-      </c>
-      <c r="P2" s="21" t="s">
-        <v>62</v>
-      </c>
-      <c r="Q2" s="21" t="s">
-        <v>62</v>
-      </c>
-      <c r="R2" s="21" t="s">
-        <v>62</v>
-      </c>
-      <c r="S2" s="22" t="s">
-        <v>62</v>
-      </c>
-      <c r="T2" s="21" t="s">
-        <v>62</v>
-      </c>
-      <c r="U2" s="21" t="s">
-        <v>62</v>
-      </c>
-      <c r="V2" s="21" t="s">
-        <v>62</v>
-      </c>
-      <c r="W2" s="21" t="s">
-        <v>62</v>
-      </c>
-      <c r="X2" s="21" t="s">
-        <v>62</v>
-      </c>
-      <c r="Y2" s="21" t="s">
-        <v>62</v>
-      </c>
-      <c r="Z2" s="21" t="s">
-        <v>62</v>
-      </c>
-      <c r="AA2" s="21" t="s">
-        <v>62</v>
-      </c>
-      <c r="AB2" s="21" t="s">
-        <v>62</v>
-      </c>
-      <c r="AC2" s="21" t="s">
-        <v>62</v>
-      </c>
-      <c r="AD2" s="21" t="s">
-        <v>62</v>
-      </c>
-      <c r="AE2" s="21" t="s">
-        <v>62</v>
-      </c>
-      <c r="AF2" s="21" t="s">
-        <v>62</v>
-      </c>
-      <c r="AG2" s="21" t="s">
-        <v>62</v>
-      </c>
-      <c r="AH2" s="21" t="s">
-        <v>62</v>
-      </c>
-      <c r="AI2" s="23" t="s">
-        <v>62</v>
-      </c>
-      <c r="AJ2" s="21" t="s">
-        <v>62</v>
-      </c>
-      <c r="AK2" s="21" t="s">
-        <v>62</v>
-      </c>
-      <c r="AL2" s="21" t="s">
-        <v>62</v>
-      </c>
-      <c r="AM2" s="21" t="s">
-        <v>62</v>
-      </c>
-      <c r="AN2" s="22" t="s">
-        <v>62</v>
-      </c>
-      <c r="AO2" s="21" t="s">
-        <v>62</v>
-      </c>
-      <c r="AP2" s="21" t="s">
-        <v>62</v>
-      </c>
-      <c r="AQ2" s="21" t="s">
-        <v>62</v>
-      </c>
-      <c r="AR2" s="21" t="s">
-        <v>62</v>
-      </c>
-      <c r="AS2" s="21" t="s">
-        <v>62</v>
-      </c>
-      <c r="AT2" s="24" t="s">
-        <v>62</v>
-      </c>
-      <c r="AU2" s="21" t="s">
-        <v>62</v>
-      </c>
-      <c r="AV2" s="22" t="s">
-        <v>62</v>
-      </c>
-      <c r="AW2" s="21" t="s">
-        <v>62</v>
-      </c>
-      <c r="AX2" s="21" t="s">
-        <v>62</v>
-      </c>
-      <c r="AY2" s="21" t="s">
-        <v>62</v>
+      <c r="A2" s="44">
+        <v>0</v>
+      </c>
+      <c r="N2" s="14"/>
+      <c r="S2" s="14"/>
+      <c r="AB2">
+        <v>13</v>
+      </c>
+      <c r="AC2">
+        <v>14</v>
+      </c>
+      <c r="AD2">
+        <v>16</v>
+      </c>
+      <c r="AE2">
+        <v>18</v>
+      </c>
+      <c r="AF2">
+        <v>20</v>
+      </c>
+      <c r="AI2" s="14"/>
+      <c r="AN2" s="14"/>
+      <c r="AR2">
+        <v>14</v>
+      </c>
+      <c r="AS2">
+        <v>15</v>
+      </c>
+      <c r="AT2" s="16">
+        <v>16</v>
+      </c>
+      <c r="AU2">
+        <v>18</v>
+      </c>
+      <c r="AV2" s="14">
+        <v>20</v>
       </c>
     </row>
     <row r="3" spans="1:51" x14ac:dyDescent="0.35">
-      <c r="A3" s="21">
-        <v>0</v>
+      <c r="A3" s="44">
+        <v>1</v>
       </c>
       <c r="N3" s="14"/>
       <c r="S3" s="14"/>
@@ -9777,8 +9638,8 @@
       </c>
     </row>
     <row r="4" spans="1:51" x14ac:dyDescent="0.35">
-      <c r="A4" s="21">
-        <v>1</v>
+      <c r="A4" s="44">
+        <v>2</v>
       </c>
       <c r="N4" s="14"/>
       <c r="S4" s="14"/>
@@ -9816,8 +9677,8 @@
       </c>
     </row>
     <row r="5" spans="1:51" x14ac:dyDescent="0.35">
-      <c r="A5" s="21">
-        <v>2</v>
+      <c r="A5" s="44">
+        <v>3</v>
       </c>
       <c r="N5" s="14"/>
       <c r="S5" s="14"/>
@@ -9855,8 +9716,8 @@
       </c>
     </row>
     <row r="6" spans="1:51" x14ac:dyDescent="0.35">
-      <c r="A6" s="21">
-        <v>3</v>
+      <c r="A6" s="44">
+        <v>4</v>
       </c>
       <c r="N6" s="14"/>
       <c r="S6" s="14"/>
@@ -9894,8 +9755,8 @@
       </c>
     </row>
     <row r="7" spans="1:51" x14ac:dyDescent="0.35">
-      <c r="A7" s="21">
-        <v>4</v>
+      <c r="A7" s="44">
+        <v>5</v>
       </c>
       <c r="N7" s="14"/>
       <c r="S7" s="14"/>
@@ -9933,8 +9794,8 @@
       </c>
     </row>
     <row r="8" spans="1:51" x14ac:dyDescent="0.35">
-      <c r="A8" s="21">
-        <v>5</v>
+      <c r="A8" s="44">
+        <v>6</v>
       </c>
       <c r="N8" s="14"/>
       <c r="S8" s="14"/>
@@ -9970,10 +9831,13 @@
       <c r="AV8" s="14">
         <v>20</v>
       </c>
+      <c r="AW8" s="25">
+        <v>33</v>
+      </c>
     </row>
     <row r="9" spans="1:51" x14ac:dyDescent="0.35">
-      <c r="A9" s="21">
-        <v>6</v>
+      <c r="A9" s="44">
+        <v>7</v>
       </c>
       <c r="N9" s="14"/>
       <c r="S9" s="14"/>
@@ -9981,41 +9845,55 @@
         <v>13</v>
       </c>
       <c r="AC9">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="AD9">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="AE9">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="AF9">
-        <v>20</v>
-      </c>
-      <c r="AI9" s="14"/>
+        <v>21</v>
+      </c>
+      <c r="AG9">
+        <v>25</v>
+      </c>
+      <c r="AH9">
+        <v>29</v>
+      </c>
+      <c r="AI9" s="14">
+        <v>33</v>
+      </c>
       <c r="AN9" s="14"/>
       <c r="AR9">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="AS9">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="AT9" s="16">
-        <v>16</v>
+        <v>18</v>
       </c>
       <c r="AU9">
-        <v>18</v>
+        <v>20</v>
       </c>
       <c r="AV9" s="14">
-        <v>20</v>
+        <v>22</v>
       </c>
       <c r="AW9" s="25">
-        <v>33</v>
+        <v>26</v>
+      </c>
+      <c r="AX9">
+        <v>30</v>
+      </c>
+      <c r="AY9">
+        <v>34</v>
       </c>
     </row>
     <row r="10" spans="1:51" x14ac:dyDescent="0.35">
-      <c r="A10" s="21">
-        <v>7</v>
+      <c r="A10" s="44">
+        <v>8</v>
       </c>
       <c r="N10" s="14"/>
       <c r="S10" s="14"/>
@@ -10059,7 +9937,7 @@
       <c r="AV10" s="14">
         <v>22</v>
       </c>
-      <c r="AW10" s="25">
+      <c r="AW10">
         <v>26</v>
       </c>
       <c r="AX10">
@@ -10070,8 +9948,8 @@
       </c>
     </row>
     <row r="11" spans="1:51" x14ac:dyDescent="0.35">
-      <c r="A11" s="21">
-        <v>8</v>
+      <c r="A11" s="44">
+        <v>9</v>
       </c>
       <c r="N11" s="14"/>
       <c r="S11" s="14"/>
@@ -10126,8 +10004,8 @@
       </c>
     </row>
     <row r="12" spans="1:51" x14ac:dyDescent="0.35">
-      <c r="A12" s="21">
-        <v>9</v>
+      <c r="A12" s="44">
+        <v>10</v>
       </c>
       <c r="N12" s="14"/>
       <c r="S12" s="14"/>
@@ -10182,8 +10060,8 @@
       </c>
     </row>
     <row r="13" spans="1:51" x14ac:dyDescent="0.35">
-      <c r="A13" s="21">
-        <v>10</v>
+      <c r="A13" s="44">
+        <v>11</v>
       </c>
       <c r="N13" s="14"/>
       <c r="S13" s="14"/>
@@ -10238,8 +10116,8 @@
       </c>
     </row>
     <row r="14" spans="1:51" x14ac:dyDescent="0.35">
-      <c r="A14" s="21">
-        <v>11</v>
+      <c r="A14" s="44">
+        <v>12</v>
       </c>
       <c r="N14" s="14"/>
       <c r="S14" s="14"/>
@@ -10294,8 +10172,8 @@
       </c>
     </row>
     <row r="15" spans="1:51" x14ac:dyDescent="0.35">
-      <c r="A15" s="21">
-        <v>12</v>
+      <c r="A15" s="44">
+        <v>13</v>
       </c>
       <c r="N15" s="14"/>
       <c r="S15" s="14"/>
@@ -10350,8 +10228,8 @@
       </c>
     </row>
     <row r="16" spans="1:51" x14ac:dyDescent="0.35">
-      <c r="A16" s="21">
-        <v>13</v>
+      <c r="A16" s="44">
+        <v>14</v>
       </c>
       <c r="N16" s="14"/>
       <c r="S16" s="14"/>
@@ -10406,8 +10284,8 @@
       </c>
     </row>
     <row r="17" spans="1:51" x14ac:dyDescent="0.35">
-      <c r="A17" s="21">
-        <v>14</v>
+      <c r="A17" s="44">
+        <v>15</v>
       </c>
       <c r="N17" s="14"/>
       <c r="S17" s="14"/>
@@ -10462,64 +10340,64 @@
       </c>
     </row>
     <row r="18" spans="1:51" x14ac:dyDescent="0.35">
-      <c r="A18" s="21">
-        <v>15</v>
+      <c r="A18" s="44">
+        <v>16</v>
       </c>
       <c r="N18" s="14"/>
       <c r="S18" s="14"/>
       <c r="AB18">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="AC18">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="AD18">
-        <v>17</v>
+        <v>19</v>
       </c>
       <c r="AE18">
-        <v>19</v>
+        <v>21</v>
       </c>
       <c r="AF18">
-        <v>21</v>
+        <v>23</v>
       </c>
       <c r="AG18">
-        <v>25</v>
+        <v>27</v>
       </c>
       <c r="AH18">
-        <v>29</v>
+        <v>31</v>
       </c>
       <c r="AI18" s="14">
-        <v>33</v>
+        <v>35</v>
       </c>
       <c r="AN18" s="14"/>
       <c r="AR18">
-        <v>15</v>
+        <v>18</v>
       </c>
       <c r="AS18">
-        <v>16</v>
+        <v>21</v>
       </c>
       <c r="AT18" s="16">
-        <v>18</v>
+        <v>24</v>
       </c>
       <c r="AU18">
-        <v>20</v>
+        <v>29</v>
       </c>
       <c r="AV18" s="14">
-        <v>22</v>
+        <v>34</v>
       </c>
       <c r="AW18">
-        <v>26</v>
+        <v>42</v>
       </c>
       <c r="AX18">
-        <v>30</v>
+        <v>51</v>
       </c>
       <c r="AY18">
-        <v>34</v>
+        <v>59</v>
       </c>
     </row>
     <row r="19" spans="1:51" x14ac:dyDescent="0.35">
-      <c r="A19" s="21">
-        <v>16</v>
+      <c r="A19" s="44">
+        <v>17</v>
       </c>
       <c r="N19" s="14"/>
       <c r="S19" s="14"/>
@@ -10574,11 +10452,87 @@
       </c>
     </row>
     <row r="20" spans="1:51" x14ac:dyDescent="0.35">
-      <c r="A20" s="21">
+      <c r="A20" s="44">
+        <v>18</v>
+      </c>
+      <c r="B20">
+        <v>16</v>
+      </c>
+      <c r="C20">
         <v>17</v>
       </c>
-      <c r="N20" s="14"/>
-      <c r="S20" s="14"/>
+      <c r="D20">
+        <v>19</v>
+      </c>
+      <c r="E20">
+        <v>23</v>
+      </c>
+      <c r="F20">
+        <v>27</v>
+      </c>
+      <c r="G20">
+        <v>35</v>
+      </c>
+      <c r="H20">
+        <v>41</v>
+      </c>
+      <c r="I20">
+        <v>51</v>
+      </c>
+      <c r="J20">
+        <v>60</v>
+      </c>
+      <c r="K20">
+        <v>66</v>
+      </c>
+      <c r="L20">
+        <v>73</v>
+      </c>
+      <c r="M20">
+        <v>80</v>
+      </c>
+      <c r="N20" s="14">
+        <v>86</v>
+      </c>
+      <c r="O20">
+        <v>20</v>
+      </c>
+      <c r="P20">
+        <v>24</v>
+      </c>
+      <c r="Q20">
+        <v>28</v>
+      </c>
+      <c r="R20">
+        <v>31</v>
+      </c>
+      <c r="S20" s="14">
+        <v>34</v>
+      </c>
+      <c r="T20">
+        <v>41</v>
+      </c>
+      <c r="U20">
+        <v>49</v>
+      </c>
+      <c r="V20">
+        <v>58</v>
+      </c>
+      <c r="W20">
+        <v>67</v>
+      </c>
+      <c r="X20">
+        <v>75</v>
+      </c>
+      <c r="Y20">
+        <v>83</v>
+      </c>
+      <c r="Z20">
+        <v>91</v>
+      </c>
+      <c r="AA20">
+        <v>99</v>
+      </c>
       <c r="AB20">
         <v>14</v>
       </c>
@@ -10630,8 +10584,8 @@
       </c>
     </row>
     <row r="21" spans="1:51" x14ac:dyDescent="0.35">
-      <c r="A21" s="21">
-        <v>18</v>
+      <c r="A21" s="44">
+        <v>19</v>
       </c>
       <c r="B21">
         <v>16</v>
@@ -10762,8 +10716,8 @@
       </c>
     </row>
     <row r="22" spans="1:51" x14ac:dyDescent="0.35">
-      <c r="A22" s="21">
-        <v>19</v>
+      <c r="A22" s="44">
+        <v>20</v>
       </c>
       <c r="B22">
         <v>16</v>
@@ -10894,8 +10848,8 @@
       </c>
     </row>
     <row r="23" spans="1:51" x14ac:dyDescent="0.35">
-      <c r="A23" s="21">
-        <v>20</v>
+      <c r="A23" s="44">
+        <v>21</v>
       </c>
       <c r="B23">
         <v>16</v>
@@ -11001,33 +10955,33 @@
       </c>
       <c r="AN23" s="14"/>
       <c r="AR23">
-        <v>18</v>
+        <v>21</v>
       </c>
       <c r="AS23">
-        <v>21</v>
+        <v>25</v>
       </c>
       <c r="AT23" s="16">
-        <v>24</v>
+        <v>30</v>
       </c>
       <c r="AU23">
-        <v>29</v>
+        <v>38</v>
       </c>
       <c r="AV23" s="14">
-        <v>34</v>
+        <v>45</v>
       </c>
       <c r="AW23">
-        <v>42</v>
+        <v>59</v>
       </c>
       <c r="AX23">
-        <v>51</v>
+        <v>73</v>
       </c>
       <c r="AY23">
-        <v>59</v>
+        <v>87</v>
       </c>
     </row>
     <row r="24" spans="1:51" x14ac:dyDescent="0.35">
-      <c r="A24" s="21">
-        <v>21</v>
+      <c r="A24" s="44">
+        <v>22</v>
       </c>
       <c r="B24">
         <v>16</v>
@@ -11158,8 +11112,8 @@
       </c>
     </row>
     <row r="25" spans="1:51" x14ac:dyDescent="0.35">
-      <c r="A25" s="21">
-        <v>22</v>
+      <c r="A25" s="44">
+        <v>23</v>
       </c>
       <c r="B25">
         <v>16</v>
@@ -11290,8 +11244,8 @@
       </c>
     </row>
     <row r="26" spans="1:51" x14ac:dyDescent="0.35">
-      <c r="A26" s="21">
-        <v>23</v>
+      <c r="A26" s="44">
+        <v>24</v>
       </c>
       <c r="B26">
         <v>16</v>
@@ -11422,8 +11376,8 @@
       </c>
     </row>
     <row r="27" spans="1:51" x14ac:dyDescent="0.35">
-      <c r="A27" s="21">
-        <v>24</v>
+      <c r="A27" s="44">
+        <v>25</v>
       </c>
       <c r="B27">
         <v>16</v>
@@ -11554,47 +11508,47 @@
       </c>
     </row>
     <row r="28" spans="1:51" x14ac:dyDescent="0.35">
-      <c r="A28" s="21">
-        <v>25</v>
+      <c r="A28" s="44">
+        <v>26</v>
       </c>
       <c r="B28">
         <v>16</v>
       </c>
       <c r="C28">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="D28">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="E28">
-        <v>23</v>
+        <v>25</v>
       </c>
       <c r="F28">
-        <v>27</v>
+        <v>29</v>
       </c>
       <c r="G28">
-        <v>35</v>
+        <v>38</v>
       </c>
       <c r="H28">
-        <v>41</v>
+        <v>46</v>
       </c>
       <c r="I28">
-        <v>51</v>
+        <v>57</v>
       </c>
       <c r="J28">
-        <v>60</v>
+        <v>68</v>
       </c>
       <c r="K28">
-        <v>66</v>
+        <v>76</v>
       </c>
       <c r="L28">
-        <v>73</v>
+        <v>84</v>
       </c>
       <c r="M28">
-        <v>80</v>
+        <v>92</v>
       </c>
       <c r="N28" s="14">
-        <v>86</v>
+        <v>100</v>
       </c>
       <c r="O28">
         <v>20</v>
@@ -11603,91 +11557,91 @@
         <v>24</v>
       </c>
       <c r="Q28">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="R28">
+        <v>32</v>
+      </c>
+      <c r="S28" s="14">
+        <v>36</v>
+      </c>
+      <c r="T28">
+        <v>43</v>
+      </c>
+      <c r="U28">
+        <v>52</v>
+      </c>
+      <c r="V28">
+        <v>62</v>
+      </c>
+      <c r="W28">
+        <v>71</v>
+      </c>
+      <c r="X28">
+        <v>80</v>
+      </c>
+      <c r="Y28">
+        <v>88</v>
+      </c>
+      <c r="Z28">
+        <v>97</v>
+      </c>
+      <c r="AA28">
+        <v>105</v>
+      </c>
+      <c r="AI28" s="14"/>
+      <c r="AJ28">
+        <v>26</v>
+      </c>
+      <c r="AK28">
+        <v>30</v>
+      </c>
+      <c r="AL28">
+        <v>35</v>
+      </c>
+      <c r="AM28">
+        <v>42</v>
+      </c>
+      <c r="AN28" s="14">
+        <v>50</v>
+      </c>
+      <c r="AO28">
+        <v>62</v>
+      </c>
+      <c r="AP28">
+        <v>85</v>
+      </c>
+      <c r="AQ28">
+        <v>102</v>
+      </c>
+      <c r="AR28">
+        <v>25</v>
+      </c>
+      <c r="AS28">
         <v>31</v>
       </c>
-      <c r="S28" s="14">
-        <v>34</v>
-      </c>
-      <c r="T28">
-        <v>41</v>
-      </c>
-      <c r="U28">
+      <c r="AT28" s="16">
+        <v>37</v>
+      </c>
+      <c r="AU28">
         <v>49</v>
       </c>
-      <c r="V28">
-        <v>58</v>
-      </c>
-      <c r="W28">
-        <v>67</v>
-      </c>
-      <c r="X28">
-        <v>75</v>
-      </c>
-      <c r="Y28">
-        <v>83</v>
-      </c>
-      <c r="Z28">
-        <v>91</v>
-      </c>
-      <c r="AA28">
-        <v>99</v>
-      </c>
-      <c r="AB28">
-        <v>14</v>
-      </c>
-      <c r="AC28">
-        <v>16</v>
-      </c>
-      <c r="AD28">
-        <v>19</v>
-      </c>
-      <c r="AE28">
-        <v>21</v>
-      </c>
-      <c r="AF28">
-        <v>23</v>
-      </c>
-      <c r="AG28">
+      <c r="AV28" s="14">
+        <v>60</v>
+      </c>
+      <c r="AW28">
+        <v>81</v>
+      </c>
+      <c r="AX28">
+        <v>102</v>
+      </c>
+      <c r="AY28">
+        <v>124</v>
+      </c>
+    </row>
+    <row r="29" spans="1:51" x14ac:dyDescent="0.35">
+      <c r="A29" s="44">
         <v>27</v>
-      </c>
-      <c r="AH28">
-        <v>31</v>
-      </c>
-      <c r="AI28" s="14">
-        <v>35</v>
-      </c>
-      <c r="AN28" s="14"/>
-      <c r="AR28">
-        <v>21</v>
-      </c>
-      <c r="AS28">
-        <v>25</v>
-      </c>
-      <c r="AT28" s="16">
-        <v>30</v>
-      </c>
-      <c r="AU28">
-        <v>38</v>
-      </c>
-      <c r="AV28" s="14">
-        <v>45</v>
-      </c>
-      <c r="AW28">
-        <v>59</v>
-      </c>
-      <c r="AX28">
-        <v>73</v>
-      </c>
-      <c r="AY28">
-        <v>87</v>
-      </c>
-    </row>
-    <row r="29" spans="1:51" x14ac:dyDescent="0.35">
-      <c r="A29" s="21">
-        <v>26</v>
       </c>
       <c r="B29">
         <v>16</v>
@@ -11818,8 +11772,8 @@
       </c>
     </row>
     <row r="30" spans="1:51" x14ac:dyDescent="0.35">
-      <c r="A30" s="21">
-        <v>27</v>
+      <c r="A30" s="44">
+        <v>28</v>
       </c>
       <c r="B30">
         <v>16</v>
@@ -11950,8 +11904,8 @@
       </c>
     </row>
     <row r="31" spans="1:51" x14ac:dyDescent="0.35">
-      <c r="A31" s="21">
-        <v>28</v>
+      <c r="A31" s="44">
+        <v>29</v>
       </c>
       <c r="B31">
         <v>16</v>
@@ -12082,8 +12036,8 @@
       </c>
     </row>
     <row r="32" spans="1:51" x14ac:dyDescent="0.35">
-      <c r="A32" s="21">
-        <v>29</v>
+      <c r="A32" s="44">
+        <v>30</v>
       </c>
       <c r="B32">
         <v>16</v>
@@ -12214,140 +12168,140 @@
       </c>
     </row>
     <row r="33" spans="1:51" x14ac:dyDescent="0.35">
-      <c r="A33" s="21">
-        <v>30</v>
+      <c r="A33" s="44">
+        <v>31</v>
       </c>
       <c r="B33">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="C33">
         <v>18</v>
       </c>
       <c r="D33">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="E33">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="F33">
-        <v>29</v>
+        <v>31</v>
       </c>
       <c r="G33">
-        <v>38</v>
+        <v>42</v>
       </c>
       <c r="H33">
-        <v>46</v>
+        <v>50</v>
       </c>
       <c r="I33">
+        <v>64</v>
+      </c>
+      <c r="J33">
+        <v>76</v>
+      </c>
+      <c r="K33">
+        <v>85</v>
+      </c>
+      <c r="L33">
+        <v>94</v>
+      </c>
+      <c r="M33">
+        <v>104</v>
+      </c>
+      <c r="N33" s="14">
+        <v>113</v>
+      </c>
+      <c r="O33">
+        <v>21</v>
+      </c>
+      <c r="P33">
+        <v>26</v>
+      </c>
+      <c r="Q33">
+        <v>30</v>
+      </c>
+      <c r="R33">
+        <v>34</v>
+      </c>
+      <c r="S33" s="14">
+        <v>39</v>
+      </c>
+      <c r="T33">
+        <v>47</v>
+      </c>
+      <c r="U33">
         <v>57</v>
       </c>
-      <c r="J33">
-        <v>68</v>
-      </c>
-      <c r="K33">
-        <v>76</v>
-      </c>
-      <c r="L33">
-        <v>84</v>
-      </c>
-      <c r="M33">
-        <v>92</v>
-      </c>
-      <c r="N33" s="14">
+      <c r="V33">
+        <v>69</v>
+      </c>
+      <c r="W33">
+        <v>80</v>
+      </c>
+      <c r="X33">
+        <v>90</v>
+      </c>
+      <c r="Y33">
         <v>100</v>
       </c>
-      <c r="O33">
-        <v>20</v>
-      </c>
-      <c r="P33">
-        <v>24</v>
-      </c>
-      <c r="Q33">
-        <v>29</v>
-      </c>
-      <c r="R33">
-        <v>32</v>
-      </c>
-      <c r="S33" s="14">
-        <v>36</v>
-      </c>
-      <c r="T33">
-        <v>43</v>
-      </c>
-      <c r="U33">
-        <v>52</v>
-      </c>
-      <c r="V33">
-        <v>62</v>
-      </c>
-      <c r="W33">
-        <v>71</v>
-      </c>
-      <c r="X33">
-        <v>80</v>
-      </c>
-      <c r="Y33">
-        <v>88</v>
-      </c>
       <c r="Z33">
-        <v>97</v>
+        <v>110</v>
       </c>
       <c r="AA33">
-        <v>105</v>
+        <v>120</v>
       </c>
       <c r="AI33" s="14"/>
       <c r="AJ33">
         <v>26</v>
       </c>
       <c r="AK33">
-        <v>30</v>
+        <v>31</v>
       </c>
       <c r="AL33">
         <v>35</v>
       </c>
       <c r="AM33">
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="AN33" s="14">
-        <v>50</v>
+        <v>51</v>
       </c>
       <c r="AO33">
-        <v>62</v>
+        <v>63</v>
       </c>
       <c r="AP33">
-        <v>85</v>
+        <v>86</v>
       </c>
       <c r="AQ33">
-        <v>102</v>
+        <v>104</v>
       </c>
       <c r="AR33">
-        <v>25</v>
+        <v>28</v>
       </c>
       <c r="AS33">
-        <v>31</v>
+        <v>36</v>
       </c>
       <c r="AT33" s="16">
-        <v>37</v>
+        <v>44</v>
       </c>
       <c r="AU33">
-        <v>49</v>
+        <v>58</v>
       </c>
       <c r="AV33" s="14">
-        <v>60</v>
+        <v>72</v>
       </c>
       <c r="AW33">
-        <v>81</v>
+        <v>99</v>
       </c>
       <c r="AX33">
-        <v>102</v>
+        <v>126</v>
       </c>
       <c r="AY33">
-        <v>124</v>
+        <v>153</v>
       </c>
     </row>
     <row r="34" spans="1:51" x14ac:dyDescent="0.35">
-      <c r="A34" s="21">
-        <v>31</v>
+      <c r="A34" s="44">
+        <v>32</v>
       </c>
       <c r="B34">
         <v>17</v>
@@ -12478,8 +12432,8 @@
       </c>
     </row>
     <row r="35" spans="1:51" x14ac:dyDescent="0.35">
-      <c r="A35" s="21">
-        <v>32</v>
+      <c r="A35" s="44">
+        <v>33</v>
       </c>
       <c r="B35">
         <v>17</v>
@@ -12610,8 +12564,8 @@
       </c>
     </row>
     <row r="36" spans="1:51" x14ac:dyDescent="0.35">
-      <c r="A36" s="21">
-        <v>33</v>
+      <c r="A36" s="44">
+        <v>34</v>
       </c>
       <c r="B36">
         <v>17</v>
@@ -12742,8 +12696,8 @@
       </c>
     </row>
     <row r="37" spans="1:51" x14ac:dyDescent="0.35">
-      <c r="A37" s="21">
-        <v>34</v>
+      <c r="A37" s="44">
+        <v>35</v>
       </c>
       <c r="B37">
         <v>17</v>
@@ -12874,86 +12828,86 @@
       </c>
     </row>
     <row r="38" spans="1:51" x14ac:dyDescent="0.35">
-      <c r="A38" s="21">
-        <v>35</v>
+      <c r="A38" s="44">
+        <v>36</v>
       </c>
       <c r="B38">
         <v>17</v>
       </c>
       <c r="C38">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="D38">
         <v>21</v>
       </c>
       <c r="E38">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="F38">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="G38">
+        <v>44</v>
+      </c>
+      <c r="H38">
+        <v>54</v>
+      </c>
+      <c r="I38">
+        <v>68</v>
+      </c>
+      <c r="J38">
+        <v>81</v>
+      </c>
+      <c r="K38">
+        <v>91</v>
+      </c>
+      <c r="L38">
+        <v>101</v>
+      </c>
+      <c r="M38">
+        <v>112</v>
+      </c>
+      <c r="N38" s="14">
+        <v>122</v>
+      </c>
+      <c r="O38">
+        <v>22</v>
+      </c>
+      <c r="P38">
+        <v>27</v>
+      </c>
+      <c r="Q38">
+        <v>32</v>
+      </c>
+      <c r="R38">
+        <v>36</v>
+      </c>
+      <c r="S38" s="14">
         <v>42</v>
       </c>
-      <c r="H38">
-        <v>50</v>
-      </c>
-      <c r="I38">
-        <v>64</v>
-      </c>
-      <c r="J38">
-        <v>76</v>
-      </c>
-      <c r="K38">
-        <v>85</v>
-      </c>
-      <c r="L38">
-        <v>94</v>
-      </c>
-      <c r="M38">
-        <v>104</v>
-      </c>
-      <c r="N38" s="14">
+      <c r="T38">
+        <v>52</v>
+      </c>
+      <c r="U38">
+        <v>63</v>
+      </c>
+      <c r="V38">
+        <v>77</v>
+      </c>
+      <c r="W38">
+        <v>90</v>
+      </c>
+      <c r="X38">
+        <v>101</v>
+      </c>
+      <c r="Y38">
         <v>113</v>
       </c>
-      <c r="O38">
-        <v>21</v>
-      </c>
-      <c r="P38">
-        <v>26</v>
-      </c>
-      <c r="Q38">
-        <v>30</v>
-      </c>
-      <c r="R38">
-        <v>34</v>
-      </c>
-      <c r="S38" s="14">
-        <v>39</v>
-      </c>
-      <c r="T38">
-        <v>47</v>
-      </c>
-      <c r="U38">
-        <v>57</v>
-      </c>
-      <c r="V38">
-        <v>69</v>
-      </c>
-      <c r="W38">
-        <v>80</v>
-      </c>
-      <c r="X38">
-        <v>90</v>
-      </c>
-      <c r="Y38">
-        <v>100</v>
-      </c>
       <c r="Z38">
-        <v>110</v>
+        <v>124</v>
       </c>
       <c r="AA38">
-        <v>120</v>
+        <v>136</v>
       </c>
       <c r="AI38" s="14"/>
       <c r="AJ38">
@@ -12963,22 +12917,22 @@
         <v>31</v>
       </c>
       <c r="AL38">
-        <v>35</v>
+        <v>36</v>
       </c>
       <c r="AM38">
-        <v>43</v>
+        <v>44</v>
       </c>
       <c r="AN38" s="14">
-        <v>51</v>
+        <v>53</v>
       </c>
       <c r="AO38">
-        <v>63</v>
+        <v>65</v>
       </c>
       <c r="AP38">
-        <v>86</v>
+        <v>90</v>
       </c>
       <c r="AQ38">
-        <v>104</v>
+        <v>107</v>
       </c>
       <c r="AR38">
         <v>28</v>
@@ -12990,24 +12944,24 @@
         <v>44</v>
       </c>
       <c r="AU38">
-        <v>58</v>
+        <v>59</v>
       </c>
       <c r="AV38" s="14">
-        <v>72</v>
+        <v>73</v>
       </c>
       <c r="AW38">
-        <v>99</v>
+        <v>100</v>
       </c>
       <c r="AX38">
-        <v>126</v>
+        <v>127</v>
       </c>
       <c r="AY38">
-        <v>153</v>
+        <v>154</v>
       </c>
     </row>
     <row r="39" spans="1:51" x14ac:dyDescent="0.35">
-      <c r="A39" s="21">
-        <v>36</v>
+      <c r="A39" s="44">
+        <v>37</v>
       </c>
       <c r="B39">
         <v>17</v>
@@ -13138,8 +13092,8 @@
       </c>
     </row>
     <row r="40" spans="1:51" x14ac:dyDescent="0.35">
-      <c r="A40" s="21">
-        <v>37</v>
+      <c r="A40" s="44">
+        <v>38</v>
       </c>
       <c r="B40">
         <v>17</v>
@@ -13270,8 +13224,8 @@
       </c>
     </row>
     <row r="41" spans="1:51" x14ac:dyDescent="0.35">
-      <c r="A41" s="21">
-        <v>38</v>
+      <c r="A41" s="44">
+        <v>39</v>
       </c>
       <c r="B41">
         <v>17</v>
@@ -13402,8 +13356,8 @@
       </c>
     </row>
     <row r="42" spans="1:51" x14ac:dyDescent="0.35">
-      <c r="A42" s="21">
-        <v>39</v>
+      <c r="A42" s="44">
+        <v>40</v>
       </c>
       <c r="B42">
         <v>17</v>
@@ -13534,8 +13488,8 @@
       </c>
     </row>
     <row r="43" spans="1:51" x14ac:dyDescent="0.35">
-      <c r="A43" s="21">
-        <v>40</v>
+      <c r="A43" s="44">
+        <v>41</v>
       </c>
       <c r="B43">
         <v>17</v>
@@ -13544,130 +13498,130 @@
         <v>19</v>
       </c>
       <c r="D43">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="E43">
-        <v>27</v>
+        <v>29</v>
       </c>
       <c r="F43">
-        <v>32</v>
+        <v>34</v>
       </c>
       <c r="G43">
-        <v>44</v>
+        <v>47</v>
       </c>
       <c r="H43">
-        <v>54</v>
+        <v>58</v>
       </c>
       <c r="I43">
-        <v>68</v>
+        <v>74</v>
       </c>
       <c r="J43">
-        <v>81</v>
+        <v>89</v>
       </c>
       <c r="K43">
-        <v>91</v>
+        <v>100</v>
       </c>
       <c r="L43">
-        <v>101</v>
+        <v>112</v>
       </c>
       <c r="M43">
-        <v>112</v>
+        <v>123</v>
       </c>
       <c r="N43" s="14">
-        <v>122</v>
+        <v>135</v>
       </c>
       <c r="O43">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="P43">
-        <v>27</v>
+        <v>29</v>
       </c>
       <c r="Q43">
-        <v>32</v>
+        <v>34</v>
       </c>
       <c r="R43">
-        <v>36</v>
+        <v>40</v>
       </c>
       <c r="S43" s="14">
-        <v>42</v>
+        <v>46</v>
       </c>
       <c r="T43">
-        <v>52</v>
+        <v>58</v>
       </c>
       <c r="U43">
-        <v>63</v>
+        <v>72</v>
       </c>
       <c r="V43">
-        <v>77</v>
+        <v>88</v>
       </c>
       <c r="W43">
-        <v>90</v>
+        <v>103</v>
       </c>
       <c r="X43">
-        <v>101</v>
+        <v>117</v>
       </c>
       <c r="Y43">
-        <v>113</v>
+        <v>131</v>
       </c>
       <c r="Z43">
-        <v>124</v>
+        <v>144</v>
       </c>
       <c r="AA43">
-        <v>136</v>
+        <v>158</v>
       </c>
       <c r="AI43" s="14"/>
       <c r="AJ43">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="AK43">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="AL43">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="AM43">
-        <v>44</v>
+        <v>46</v>
       </c>
       <c r="AN43" s="14">
-        <v>53</v>
+        <v>55</v>
       </c>
       <c r="AO43">
-        <v>65</v>
+        <v>68</v>
       </c>
       <c r="AP43">
-        <v>90</v>
+        <v>94</v>
       </c>
       <c r="AQ43">
-        <v>107</v>
+        <v>113</v>
       </c>
       <c r="AR43">
         <v>28</v>
       </c>
       <c r="AS43">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="AT43" s="16">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="AU43">
-        <v>59</v>
+        <v>57</v>
       </c>
       <c r="AV43" s="14">
-        <v>73</v>
+        <v>71</v>
       </c>
       <c r="AW43">
-        <v>100</v>
+        <v>96</v>
       </c>
       <c r="AX43">
-        <v>127</v>
+        <v>123</v>
       </c>
       <c r="AY43">
-        <v>154</v>
+        <v>149</v>
       </c>
     </row>
     <row r="44" spans="1:51" x14ac:dyDescent="0.35">
-      <c r="A44" s="21">
-        <v>41</v>
+      <c r="A44" s="44">
+        <v>42</v>
       </c>
       <c r="B44">
         <v>17</v>
@@ -13798,8 +13752,8 @@
       </c>
     </row>
     <row r="45" spans="1:51" x14ac:dyDescent="0.35">
-      <c r="A45" s="21">
-        <v>42</v>
+      <c r="A45" s="44">
+        <v>43</v>
       </c>
       <c r="B45">
         <v>17</v>
@@ -13930,8 +13884,8 @@
       </c>
     </row>
     <row r="46" spans="1:51" x14ac:dyDescent="0.35">
-      <c r="A46" s="21">
-        <v>43</v>
+      <c r="A46" s="44">
+        <v>44</v>
       </c>
       <c r="B46">
         <v>17</v>
@@ -14062,8 +14016,8 @@
       </c>
     </row>
     <row r="47" spans="1:51" x14ac:dyDescent="0.35">
-      <c r="A47" s="21">
-        <v>44</v>
+      <c r="A47" s="44">
+        <v>45</v>
       </c>
       <c r="B47">
         <v>17</v>
@@ -14194,140 +14148,140 @@
       </c>
     </row>
     <row r="48" spans="1:51" x14ac:dyDescent="0.35">
-      <c r="A48" s="21">
-        <v>45</v>
+      <c r="A48" s="44">
+        <v>46</v>
       </c>
       <c r="B48">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="C48">
-        <v>19</v>
+        <v>21</v>
       </c>
       <c r="D48">
-        <v>22</v>
+        <v>24</v>
       </c>
       <c r="E48">
-        <v>29</v>
+        <v>32</v>
       </c>
       <c r="F48">
-        <v>34</v>
+        <v>39</v>
       </c>
       <c r="G48">
+        <v>55</v>
+      </c>
+      <c r="H48">
+        <v>69</v>
+      </c>
+      <c r="I48">
+        <v>89</v>
+      </c>
+      <c r="J48">
+        <v>107</v>
+      </c>
+      <c r="K48">
+        <v>121</v>
+      </c>
+      <c r="L48">
+        <v>136</v>
+      </c>
+      <c r="M48">
+        <v>150</v>
+      </c>
+      <c r="N48" s="14">
+        <v>165</v>
+      </c>
+      <c r="O48">
+        <v>25</v>
+      </c>
+      <c r="P48">
+        <v>32</v>
+      </c>
+      <c r="Q48">
+        <v>39</v>
+      </c>
+      <c r="R48">
         <v>47</v>
       </c>
-      <c r="H48">
-        <v>58</v>
-      </c>
-      <c r="I48">
-        <v>74</v>
-      </c>
-      <c r="J48">
+      <c r="S48" s="14">
+        <v>55</v>
+      </c>
+      <c r="T48">
+        <v>71</v>
+      </c>
+      <c r="U48">
         <v>89</v>
       </c>
-      <c r="K48">
-        <v>100</v>
-      </c>
-      <c r="L48">
-        <v>112</v>
-      </c>
-      <c r="M48">
-        <v>123</v>
-      </c>
-      <c r="N48" s="14">
-        <v>135</v>
-      </c>
-      <c r="O48">
-        <v>23</v>
-      </c>
-      <c r="P48">
-        <v>29</v>
-      </c>
-      <c r="Q48">
-        <v>34</v>
-      </c>
-      <c r="R48">
-        <v>40</v>
-      </c>
-      <c r="S48" s="14">
-        <v>46</v>
-      </c>
-      <c r="T48">
-        <v>58</v>
-      </c>
-      <c r="U48">
-        <v>72</v>
-      </c>
       <c r="V48">
-        <v>88</v>
+        <v>110</v>
       </c>
       <c r="W48">
-        <v>103</v>
+        <v>129</v>
       </c>
       <c r="X48">
-        <v>117</v>
+        <v>148</v>
       </c>
       <c r="Y48">
-        <v>131</v>
+        <v>166</v>
       </c>
       <c r="Z48">
-        <v>144</v>
+        <v>184</v>
       </c>
       <c r="AA48">
-        <v>158</v>
+        <v>202</v>
       </c>
       <c r="AI48" s="14"/>
       <c r="AJ48">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="AK48">
-        <v>32</v>
+        <v>34</v>
       </c>
       <c r="AL48">
-        <v>37</v>
+        <v>40</v>
       </c>
       <c r="AM48">
-        <v>46</v>
+        <v>49</v>
       </c>
       <c r="AN48" s="14">
-        <v>55</v>
+        <v>59</v>
       </c>
       <c r="AO48">
-        <v>68</v>
+        <v>74</v>
       </c>
       <c r="AP48">
-        <v>94</v>
+        <v>103</v>
       </c>
       <c r="AQ48">
-        <v>113</v>
+        <v>124</v>
       </c>
       <c r="AR48">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="AS48">
-        <v>35</v>
+        <v>36</v>
       </c>
       <c r="AT48" s="16">
-        <v>43</v>
+        <v>44</v>
       </c>
       <c r="AU48">
-        <v>57</v>
+        <v>59</v>
       </c>
       <c r="AV48" s="14">
-        <v>71</v>
+        <v>74</v>
       </c>
       <c r="AW48">
-        <v>96</v>
+        <v>101</v>
       </c>
       <c r="AX48">
-        <v>123</v>
+        <v>128</v>
       </c>
       <c r="AY48">
-        <v>149</v>
+        <v>156</v>
       </c>
     </row>
     <row r="49" spans="1:51" x14ac:dyDescent="0.35">
-      <c r="A49" s="21">
-        <v>46</v>
+      <c r="A49" s="44">
+        <v>47</v>
       </c>
       <c r="B49">
         <v>18</v>
@@ -14458,8 +14412,8 @@
       </c>
     </row>
     <row r="50" spans="1:51" x14ac:dyDescent="0.35">
-      <c r="A50" s="21">
-        <v>47</v>
+      <c r="A50" s="44">
+        <v>48</v>
       </c>
       <c r="B50">
         <v>18</v>
@@ -14590,8 +14544,8 @@
       </c>
     </row>
     <row r="51" spans="1:51" x14ac:dyDescent="0.35">
-      <c r="A51" s="21">
-        <v>48</v>
+      <c r="A51" s="44">
+        <v>49</v>
       </c>
       <c r="B51">
         <v>18</v>
@@ -14722,8 +14676,8 @@
       </c>
     </row>
     <row r="52" spans="1:51" x14ac:dyDescent="0.35">
-      <c r="A52" s="21">
-        <v>49</v>
+      <c r="A52" s="44">
+        <v>50</v>
       </c>
       <c r="B52">
         <v>18</v>
@@ -14854,140 +14808,140 @@
       </c>
     </row>
     <row r="53" spans="1:51" x14ac:dyDescent="0.35">
-      <c r="A53" s="21">
-        <v>50</v>
+      <c r="A53" s="44">
+        <v>51</v>
       </c>
       <c r="B53">
-        <v>18</v>
+        <v>20</v>
       </c>
       <c r="C53">
-        <v>21</v>
+        <v>24</v>
       </c>
       <c r="D53">
-        <v>24</v>
+        <v>28</v>
       </c>
       <c r="E53">
-        <v>32</v>
+        <v>38</v>
       </c>
       <c r="F53">
-        <v>39</v>
+        <v>48</v>
       </c>
       <c r="G53">
-        <v>55</v>
+        <v>70</v>
       </c>
       <c r="H53">
-        <v>69</v>
+        <v>88</v>
       </c>
       <c r="I53">
-        <v>89</v>
+        <v>115</v>
       </c>
       <c r="J53">
-        <v>107</v>
+        <v>139</v>
       </c>
       <c r="K53">
-        <v>121</v>
+        <v>160</v>
       </c>
       <c r="L53">
-        <v>136</v>
+        <v>180</v>
       </c>
       <c r="M53">
-        <v>150</v>
+        <v>200</v>
       </c>
       <c r="N53" s="14">
-        <v>165</v>
+        <v>220</v>
       </c>
       <c r="O53">
-        <v>25</v>
+        <v>29</v>
       </c>
       <c r="P53">
-        <v>32</v>
+        <v>38</v>
       </c>
       <c r="Q53">
-        <v>39</v>
+        <v>48</v>
       </c>
       <c r="R53">
-        <v>47</v>
+        <v>58</v>
       </c>
       <c r="S53" s="14">
-        <v>55</v>
+        <v>70</v>
       </c>
       <c r="T53">
-        <v>71</v>
+        <v>93</v>
       </c>
       <c r="U53">
-        <v>89</v>
+        <v>119</v>
       </c>
       <c r="V53">
-        <v>110</v>
+        <v>148</v>
       </c>
       <c r="W53">
-        <v>129</v>
+        <v>175</v>
       </c>
       <c r="X53">
-        <v>148</v>
+        <v>201</v>
       </c>
       <c r="Y53">
-        <v>166</v>
+        <v>227</v>
       </c>
       <c r="Z53">
-        <v>184</v>
+        <v>252</v>
       </c>
       <c r="AA53">
-        <v>202</v>
+        <v>278</v>
       </c>
       <c r="AI53" s="14"/>
       <c r="AJ53">
-        <v>28</v>
+        <v>30</v>
       </c>
       <c r="AK53">
-        <v>34</v>
+        <v>37</v>
       </c>
       <c r="AL53">
+        <v>44</v>
+      </c>
+      <c r="AM53">
+        <v>55</v>
+      </c>
+      <c r="AN53" s="14">
+        <v>67</v>
+      </c>
+      <c r="AO53">
+        <v>84</v>
+      </c>
+      <c r="AP53">
+        <v>118</v>
+      </c>
+      <c r="AQ53">
+        <v>143</v>
+      </c>
+      <c r="AR53">
+        <v>31</v>
+      </c>
+      <c r="AS53">
         <v>40</v>
       </c>
-      <c r="AM53">
-        <v>49</v>
-      </c>
-      <c r="AN53" s="14">
-        <v>59</v>
-      </c>
-      <c r="AO53">
-        <v>74</v>
-      </c>
-      <c r="AP53">
-        <v>103</v>
-      </c>
-      <c r="AQ53">
-        <v>124</v>
-      </c>
-      <c r="AR53">
-        <v>29</v>
-      </c>
-      <c r="AS53">
-        <v>36</v>
-      </c>
       <c r="AT53" s="16">
-        <v>44</v>
+        <v>50</v>
       </c>
       <c r="AU53">
-        <v>59</v>
+        <v>68</v>
       </c>
       <c r="AV53" s="14">
-        <v>74</v>
+        <v>84</v>
       </c>
       <c r="AW53">
-        <v>101</v>
+        <v>116</v>
       </c>
       <c r="AX53">
-        <v>128</v>
+        <v>149</v>
       </c>
       <c r="AY53">
-        <v>156</v>
+        <v>182</v>
       </c>
     </row>
     <row r="54" spans="1:51" x14ac:dyDescent="0.35">
-      <c r="A54" s="21">
-        <v>51</v>
+      <c r="A54" s="44">
+        <v>52</v>
       </c>
       <c r="B54">
         <v>20</v>
@@ -15118,8 +15072,8 @@
       </c>
     </row>
     <row r="55" spans="1:51" x14ac:dyDescent="0.35">
-      <c r="A55" s="21">
-        <v>52</v>
+      <c r="A55" s="44">
+        <v>53</v>
       </c>
       <c r="B55">
         <v>20</v>
@@ -15250,8 +15204,8 @@
       </c>
     </row>
     <row r="56" spans="1:51" x14ac:dyDescent="0.35">
-      <c r="A56" s="21">
-        <v>53</v>
+      <c r="A56" s="44">
+        <v>54</v>
       </c>
       <c r="B56">
         <v>20</v>
@@ -15382,8 +15336,8 @@
       </c>
     </row>
     <row r="57" spans="1:51" x14ac:dyDescent="0.35">
-      <c r="A57" s="21">
-        <v>54</v>
+      <c r="A57" s="44">
+        <v>55</v>
       </c>
       <c r="B57">
         <v>20</v>
@@ -15514,140 +15468,140 @@
       </c>
     </row>
     <row r="58" spans="1:51" x14ac:dyDescent="0.35">
-      <c r="A58" s="21">
-        <v>55</v>
+      <c r="A58" s="44">
+        <v>56</v>
       </c>
       <c r="B58">
-        <v>20</v>
+        <v>23</v>
       </c>
       <c r="C58">
-        <v>24</v>
+        <v>28</v>
       </c>
       <c r="D58">
-        <v>28</v>
+        <v>34</v>
       </c>
       <c r="E58">
-        <v>38</v>
+        <v>48</v>
       </c>
       <c r="F58">
-        <v>48</v>
+        <v>62</v>
       </c>
       <c r="G58">
-        <v>70</v>
+        <v>92</v>
       </c>
       <c r="H58">
-        <v>88</v>
+        <v>118</v>
       </c>
       <c r="I58">
-        <v>115</v>
+        <v>155</v>
       </c>
       <c r="J58">
-        <v>139</v>
+        <v>190</v>
       </c>
       <c r="K58">
-        <v>160</v>
+        <v>218</v>
       </c>
       <c r="L58">
-        <v>180</v>
+        <v>247</v>
       </c>
       <c r="M58">
-        <v>200</v>
+        <v>275</v>
       </c>
       <c r="N58" s="14">
-        <v>220</v>
+        <v>304</v>
       </c>
       <c r="O58">
-        <v>29</v>
+        <v>35</v>
       </c>
       <c r="P58">
-        <v>38</v>
+        <v>47</v>
       </c>
       <c r="Q58">
-        <v>48</v>
+        <v>60</v>
       </c>
       <c r="R58">
-        <v>58</v>
+        <v>76</v>
       </c>
       <c r="S58" s="14">
-        <v>70</v>
+        <v>93</v>
       </c>
       <c r="T58">
-        <v>93</v>
+        <v>126</v>
       </c>
       <c r="U58">
-        <v>119</v>
+        <v>163</v>
       </c>
       <c r="V58">
-        <v>148</v>
+        <v>204</v>
       </c>
       <c r="W58">
-        <v>175</v>
+        <v>244</v>
       </c>
       <c r="X58">
-        <v>201</v>
+        <v>281</v>
       </c>
       <c r="Y58">
-        <v>227</v>
+        <v>318</v>
       </c>
       <c r="Z58">
-        <v>252</v>
+        <v>354</v>
       </c>
       <c r="AA58">
-        <v>278</v>
+        <v>391</v>
       </c>
       <c r="AI58" s="14"/>
       <c r="AJ58">
-        <v>30</v>
+        <v>34</v>
       </c>
       <c r="AK58">
-        <v>37</v>
+        <v>42</v>
       </c>
       <c r="AL58">
-        <v>44</v>
+        <v>50</v>
       </c>
       <c r="AM58">
-        <v>55</v>
+        <v>63</v>
       </c>
       <c r="AN58" s="14">
-        <v>67</v>
+        <v>78</v>
       </c>
       <c r="AO58">
-        <v>84</v>
+        <v>100</v>
       </c>
       <c r="AP58">
-        <v>118</v>
+        <v>141</v>
       </c>
       <c r="AQ58">
-        <v>143</v>
+        <v>171</v>
       </c>
       <c r="AR58">
-        <v>31</v>
+        <v>36</v>
       </c>
       <c r="AS58">
-        <v>40</v>
+        <v>47</v>
       </c>
       <c r="AT58" s="16">
-        <v>50</v>
+        <v>59</v>
       </c>
       <c r="AU58">
-        <v>68</v>
+        <v>82</v>
       </c>
       <c r="AV58" s="14">
-        <v>84</v>
+        <v>103</v>
       </c>
       <c r="AW58">
-        <v>116</v>
+        <v>145</v>
       </c>
       <c r="AX58">
-        <v>149</v>
+        <v>186</v>
       </c>
       <c r="AY58">
-        <v>182</v>
+        <v>228</v>
       </c>
     </row>
     <row r="59" spans="1:51" x14ac:dyDescent="0.35">
-      <c r="A59" s="21">
-        <v>56</v>
+      <c r="A59" s="44">
+        <v>57</v>
       </c>
       <c r="B59">
         <v>23</v>
@@ -15778,8 +15732,8 @@
       </c>
     </row>
     <row r="60" spans="1:51" x14ac:dyDescent="0.35">
-      <c r="A60" s="21">
-        <v>57</v>
+      <c r="A60" s="44">
+        <v>58</v>
       </c>
       <c r="B60">
         <v>23</v>
@@ -15910,8 +15864,8 @@
       </c>
     </row>
     <row r="61" spans="1:51" x14ac:dyDescent="0.35">
-      <c r="A61" s="21">
-        <v>58</v>
+      <c r="A61" s="44">
+        <v>59</v>
       </c>
       <c r="B61">
         <v>23</v>
@@ -16042,8 +15996,8 @@
       </c>
     </row>
     <row r="62" spans="1:51" x14ac:dyDescent="0.35">
-      <c r="A62" s="21">
-        <v>59</v>
+      <c r="A62" s="44">
+        <v>60</v>
       </c>
       <c r="B62">
         <v>23</v>
@@ -16174,140 +16128,140 @@
       </c>
     </row>
     <row r="63" spans="1:51" x14ac:dyDescent="0.35">
-      <c r="A63" s="21">
+      <c r="A63" s="44">
+        <v>61</v>
+      </c>
+      <c r="B63">
+        <v>27</v>
+      </c>
+      <c r="C63">
+        <v>34</v>
+      </c>
+      <c r="D63">
+        <v>43</v>
+      </c>
+      <c r="E63">
+        <v>63</v>
+      </c>
+      <c r="F63">
+        <v>82</v>
+      </c>
+      <c r="G63">
+        <v>124</v>
+      </c>
+      <c r="H63">
+        <v>162</v>
+      </c>
+      <c r="I63">
+        <v>215</v>
+      </c>
+      <c r="J63">
+        <v>264</v>
+      </c>
+      <c r="K63">
+        <v>305</v>
+      </c>
+      <c r="L63">
+        <v>346</v>
+      </c>
+      <c r="M63">
+        <v>387</v>
+      </c>
+      <c r="N63" s="14">
+        <v>428</v>
+      </c>
+      <c r="O63">
+        <v>43</v>
+      </c>
+      <c r="P63">
         <v>60</v>
       </c>
-      <c r="B63">
-        <v>23</v>
-      </c>
-      <c r="C63">
-        <v>28</v>
-      </c>
-      <c r="D63">
-        <v>34</v>
-      </c>
-      <c r="E63">
-        <v>48</v>
-      </c>
-      <c r="F63">
-        <v>62</v>
-      </c>
-      <c r="G63">
-        <v>92</v>
-      </c>
-      <c r="H63">
-        <v>118</v>
-      </c>
-      <c r="I63">
-        <v>155</v>
-      </c>
-      <c r="J63">
-        <v>190</v>
-      </c>
-      <c r="K63">
-        <v>218</v>
-      </c>
-      <c r="L63">
-        <v>247</v>
-      </c>
-      <c r="M63">
-        <v>275</v>
-      </c>
-      <c r="N63" s="14">
-        <v>304</v>
-      </c>
-      <c r="O63">
-        <v>35</v>
-      </c>
-      <c r="P63">
-        <v>47</v>
-      </c>
       <c r="Q63">
-        <v>60</v>
+        <v>78</v>
       </c>
       <c r="R63">
-        <v>76</v>
+        <v>101</v>
       </c>
       <c r="S63" s="14">
-        <v>93</v>
+        <v>126</v>
       </c>
       <c r="T63">
-        <v>126</v>
+        <v>173</v>
       </c>
       <c r="U63">
-        <v>163</v>
+        <v>227</v>
       </c>
       <c r="V63">
-        <v>204</v>
+        <v>286</v>
       </c>
       <c r="W63">
-        <v>244</v>
+        <v>343</v>
       </c>
       <c r="X63">
-        <v>281</v>
+        <v>396</v>
       </c>
       <c r="Y63">
-        <v>318</v>
+        <v>449</v>
       </c>
       <c r="Z63">
-        <v>354</v>
+        <v>502</v>
       </c>
       <c r="AA63">
-        <v>391</v>
+        <v>556</v>
       </c>
       <c r="AI63" s="14"/>
       <c r="AJ63">
-        <v>34</v>
+        <v>39</v>
       </c>
       <c r="AK63">
-        <v>42</v>
+        <v>49</v>
       </c>
       <c r="AL63">
-        <v>50</v>
+        <v>59</v>
       </c>
       <c r="AM63">
-        <v>63</v>
+        <v>76</v>
       </c>
       <c r="AN63" s="14">
-        <v>78</v>
+        <v>95</v>
       </c>
       <c r="AO63">
-        <v>100</v>
+        <v>123</v>
       </c>
       <c r="AP63">
-        <v>141</v>
+        <v>174</v>
       </c>
       <c r="AQ63">
-        <v>171</v>
+        <v>213</v>
       </c>
       <c r="AR63">
-        <v>36</v>
+        <v>44</v>
       </c>
       <c r="AS63">
-        <v>47</v>
+        <v>59</v>
       </c>
       <c r="AT63" s="16">
-        <v>59</v>
+        <v>76</v>
       </c>
       <c r="AU63">
-        <v>82</v>
+        <v>106</v>
       </c>
       <c r="AV63" s="14">
-        <v>103</v>
+        <v>136</v>
       </c>
       <c r="AW63">
-        <v>145</v>
+        <v>192</v>
       </c>
       <c r="AX63">
-        <v>186</v>
+        <v>249</v>
       </c>
       <c r="AY63">
-        <v>228</v>
+        <v>306</v>
       </c>
     </row>
     <row r="64" spans="1:51" x14ac:dyDescent="0.35">
-      <c r="A64" s="21">
-        <v>61</v>
+      <c r="A64" s="44">
+        <v>62</v>
       </c>
       <c r="B64">
         <v>27</v>
@@ -16438,8 +16392,8 @@
       </c>
     </row>
     <row r="65" spans="1:51" x14ac:dyDescent="0.35">
-      <c r="A65" s="21">
-        <v>62</v>
+      <c r="A65" s="44">
+        <v>63</v>
       </c>
       <c r="B65">
         <v>27</v>
@@ -16570,8 +16524,8 @@
       </c>
     </row>
     <row r="66" spans="1:51" x14ac:dyDescent="0.35">
-      <c r="A66" s="21">
-        <v>63</v>
+      <c r="A66" s="44">
+        <v>64</v>
       </c>
       <c r="B66">
         <v>27</v>
@@ -16702,8 +16656,8 @@
       </c>
     </row>
     <row r="67" spans="1:51" x14ac:dyDescent="0.35">
-      <c r="A67" s="21">
-        <v>64</v>
+      <c r="A67" s="44">
+        <v>65</v>
       </c>
       <c r="B67">
         <v>27</v>
@@ -16834,140 +16788,140 @@
       </c>
     </row>
     <row r="68" spans="1:51" x14ac:dyDescent="0.35">
-      <c r="A68" s="21">
-        <v>65</v>
+      <c r="A68" s="44">
+        <v>66</v>
       </c>
       <c r="B68">
-        <v>27</v>
+        <v>33</v>
       </c>
       <c r="C68">
-        <v>34</v>
+        <v>44</v>
       </c>
       <c r="D68">
-        <v>43</v>
+        <v>56</v>
       </c>
       <c r="E68">
-        <v>63</v>
+        <v>84</v>
       </c>
       <c r="F68">
-        <v>82</v>
+        <v>111</v>
       </c>
       <c r="G68">
-        <v>124</v>
+        <v>171</v>
       </c>
       <c r="H68">
-        <v>162</v>
+        <v>226</v>
       </c>
       <c r="I68">
-        <v>215</v>
+        <v>302</v>
       </c>
       <c r="J68">
-        <v>264</v>
+        <v>372</v>
       </c>
       <c r="K68">
-        <v>305</v>
+        <v>431</v>
       </c>
       <c r="L68">
-        <v>346</v>
+        <v>490</v>
       </c>
       <c r="M68">
-        <v>387</v>
+        <v>549</v>
       </c>
       <c r="N68" s="14">
-        <v>428</v>
+        <v>608</v>
       </c>
       <c r="O68">
-        <v>43</v>
+        <v>55</v>
       </c>
       <c r="P68">
-        <v>60</v>
+        <v>79</v>
       </c>
       <c r="Q68">
-        <v>78</v>
+        <v>104</v>
       </c>
       <c r="R68">
-        <v>101</v>
+        <v>137</v>
       </c>
       <c r="S68" s="14">
-        <v>126</v>
+        <v>174</v>
       </c>
       <c r="T68">
-        <v>173</v>
+        <v>241</v>
       </c>
       <c r="U68">
-        <v>227</v>
+        <v>318</v>
       </c>
       <c r="V68">
-        <v>286</v>
+        <v>404</v>
       </c>
       <c r="W68">
-        <v>343</v>
+        <v>485</v>
       </c>
       <c r="X68">
-        <v>396</v>
+        <v>561</v>
       </c>
       <c r="Y68">
-        <v>449</v>
+        <v>637</v>
       </c>
       <c r="Z68">
-        <v>502</v>
+        <v>714</v>
       </c>
       <c r="AA68">
-        <v>556</v>
+        <v>790</v>
       </c>
       <c r="AI68" s="14"/>
       <c r="AJ68">
-        <v>39</v>
+        <v>46</v>
       </c>
       <c r="AK68">
-        <v>49</v>
+        <v>59</v>
       </c>
       <c r="AL68">
-        <v>59</v>
+        <v>72</v>
       </c>
       <c r="AM68">
-        <v>76</v>
+        <v>95</v>
       </c>
       <c r="AN68" s="14">
-        <v>95</v>
+        <v>120</v>
       </c>
       <c r="AO68">
-        <v>123</v>
+        <v>157</v>
       </c>
       <c r="AP68">
-        <v>174</v>
+        <v>223</v>
       </c>
       <c r="AQ68">
-        <v>213</v>
+        <v>273</v>
       </c>
       <c r="AR68">
-        <v>44</v>
+        <v>58</v>
       </c>
       <c r="AS68">
-        <v>59</v>
+        <v>79</v>
       </c>
       <c r="AT68" s="16">
-        <v>76</v>
+        <v>102</v>
       </c>
       <c r="AU68">
-        <v>106</v>
+        <v>145</v>
       </c>
       <c r="AV68" s="14">
-        <v>136</v>
+        <v>187</v>
       </c>
       <c r="AW68">
-        <v>192</v>
+        <v>267</v>
       </c>
       <c r="AX68">
-        <v>249</v>
+        <v>348</v>
       </c>
       <c r="AY68">
-        <v>306</v>
+        <v>429</v>
       </c>
     </row>
     <row r="69" spans="1:51" x14ac:dyDescent="0.35">
-      <c r="A69" s="21">
-        <v>66</v>
+      <c r="A69" s="44">
+        <v>67</v>
       </c>
       <c r="B69">
         <v>33</v>
@@ -17098,8 +17052,8 @@
       </c>
     </row>
     <row r="70" spans="1:51" x14ac:dyDescent="0.35">
-      <c r="A70" s="21">
-        <v>67</v>
+      <c r="A70" s="44">
+        <v>68</v>
       </c>
       <c r="B70">
         <v>33</v>
@@ -17230,8 +17184,8 @@
       </c>
     </row>
     <row r="71" spans="1:51" x14ac:dyDescent="0.35">
-      <c r="A71" s="21">
-        <v>68</v>
+      <c r="A71" s="44">
+        <v>69</v>
       </c>
       <c r="B71">
         <v>33</v>
@@ -17362,8 +17316,8 @@
       </c>
     </row>
     <row r="72" spans="1:51" x14ac:dyDescent="0.35">
-      <c r="A72" s="21">
-        <v>69</v>
+      <c r="A72" s="44">
+        <v>70</v>
       </c>
       <c r="B72">
         <v>33</v>
@@ -17494,140 +17448,140 @@
       </c>
     </row>
     <row r="73" spans="1:51" x14ac:dyDescent="0.35">
-      <c r="A73" s="21">
-        <v>70</v>
+      <c r="A73" s="44">
+        <v>71</v>
       </c>
       <c r="B73">
-        <v>33</v>
+        <v>42</v>
       </c>
       <c r="C73">
-        <v>44</v>
+        <v>57</v>
       </c>
       <c r="D73">
-        <v>56</v>
+        <v>74</v>
       </c>
       <c r="E73">
-        <v>84</v>
+        <v>113</v>
       </c>
       <c r="F73">
-        <v>111</v>
+        <v>152</v>
       </c>
       <c r="G73">
-        <v>171</v>
+        <v>238</v>
       </c>
       <c r="H73">
-        <v>226</v>
+        <v>316</v>
       </c>
       <c r="I73">
-        <v>302</v>
+        <v>423</v>
       </c>
       <c r="J73">
-        <v>372</v>
+        <v>524</v>
       </c>
       <c r="K73">
-        <v>431</v>
+        <v>608</v>
       </c>
       <c r="L73">
-        <v>490</v>
+        <v>692</v>
       </c>
       <c r="M73">
-        <v>549</v>
+        <v>776</v>
       </c>
       <c r="N73" s="14">
-        <v>608</v>
+        <v>861</v>
       </c>
       <c r="O73">
-        <v>55</v>
+        <v>72</v>
       </c>
       <c r="P73">
-        <v>79</v>
+        <v>105</v>
       </c>
       <c r="Q73">
-        <v>104</v>
+        <v>140</v>
       </c>
       <c r="R73">
-        <v>137</v>
+        <v>188</v>
       </c>
       <c r="S73" s="14">
-        <v>174</v>
+        <v>240</v>
       </c>
       <c r="T73">
-        <v>241</v>
+        <v>337</v>
       </c>
       <c r="U73">
-        <v>318</v>
+        <v>445</v>
       </c>
       <c r="V73">
-        <v>404</v>
+        <v>567</v>
       </c>
       <c r="W73">
-        <v>485</v>
+        <v>683</v>
       </c>
       <c r="X73">
-        <v>561</v>
+        <v>792</v>
       </c>
       <c r="Y73">
-        <v>637</v>
+        <v>901</v>
       </c>
       <c r="Z73">
-        <v>714</v>
+        <v>1010</v>
       </c>
       <c r="AA73">
-        <v>790</v>
+        <v>1119</v>
       </c>
       <c r="AI73" s="14"/>
       <c r="AJ73">
-        <v>46</v>
+        <v>56</v>
       </c>
       <c r="AK73">
-        <v>59</v>
+        <v>73</v>
       </c>
       <c r="AL73">
+        <v>91</v>
+      </c>
+      <c r="AM73">
+        <v>121</v>
+      </c>
+      <c r="AN73" s="14">
+        <v>155</v>
+      </c>
+      <c r="AO73">
+        <v>204</v>
+      </c>
+      <c r="AP73">
+        <v>293</v>
+      </c>
+      <c r="AQ73">
+        <v>360</v>
+      </c>
+      <c r="AR73">
+        <v>77</v>
+      </c>
+      <c r="AS73">
+        <v>107</v>
+      </c>
+      <c r="AT73" s="16">
+        <v>140</v>
+      </c>
+      <c r="AU73">
+        <v>202</v>
+      </c>
+      <c r="AV73" s="14">
+        <v>261</v>
+      </c>
+      <c r="AW73">
+        <v>376</v>
+      </c>
+      <c r="AX73">
+        <v>492</v>
+      </c>
+      <c r="AY73">
+        <v>609</v>
+      </c>
+    </row>
+    <row r="74" spans="1:51" x14ac:dyDescent="0.35">
+      <c r="A74" s="44">
         <v>72</v>
-      </c>
-      <c r="AM73">
-        <v>95</v>
-      </c>
-      <c r="AN73" s="14">
-        <v>120</v>
-      </c>
-      <c r="AO73">
-        <v>157</v>
-      </c>
-      <c r="AP73">
-        <v>223</v>
-      </c>
-      <c r="AQ73">
-        <v>273</v>
-      </c>
-      <c r="AR73">
-        <v>58</v>
-      </c>
-      <c r="AS73">
-        <v>79</v>
-      </c>
-      <c r="AT73" s="16">
-        <v>102</v>
-      </c>
-      <c r="AU73">
-        <v>145</v>
-      </c>
-      <c r="AV73" s="14">
-        <v>187</v>
-      </c>
-      <c r="AW73">
-        <v>267</v>
-      </c>
-      <c r="AX73">
-        <v>348</v>
-      </c>
-      <c r="AY73">
-        <v>429</v>
-      </c>
-    </row>
-    <row r="74" spans="1:51" x14ac:dyDescent="0.35">
-      <c r="A74" s="21">
-        <v>71</v>
       </c>
       <c r="B74">
         <v>42</v>
@@ -17758,8 +17712,8 @@
       </c>
     </row>
     <row r="75" spans="1:51" x14ac:dyDescent="0.35">
-      <c r="A75" s="21">
-        <v>72</v>
+      <c r="A75" s="44">
+        <v>73</v>
       </c>
       <c r="B75">
         <v>42</v>
@@ -17890,8 +17844,8 @@
       </c>
     </row>
     <row r="76" spans="1:51" x14ac:dyDescent="0.35">
-      <c r="A76" s="21">
-        <v>73</v>
+      <c r="A76" s="44">
+        <v>74</v>
       </c>
       <c r="B76">
         <v>42</v>
@@ -18022,8 +17976,8 @@
       </c>
     </row>
     <row r="77" spans="1:51" x14ac:dyDescent="0.35">
-      <c r="A77" s="21">
-        <v>74</v>
+      <c r="A77" s="44">
+        <v>75</v>
       </c>
       <c r="B77">
         <v>42</v>
@@ -18154,140 +18108,64 @@
       </c>
     </row>
     <row r="78" spans="1:51" x14ac:dyDescent="0.35">
-      <c r="A78" s="21">
-        <v>75</v>
-      </c>
-      <c r="B78">
-        <v>42</v>
-      </c>
-      <c r="C78">
-        <v>57</v>
-      </c>
-      <c r="D78">
-        <v>74</v>
-      </c>
-      <c r="E78">
-        <v>113</v>
-      </c>
-      <c r="F78">
-        <v>152</v>
-      </c>
-      <c r="G78">
-        <v>238</v>
-      </c>
-      <c r="H78">
-        <v>316</v>
-      </c>
-      <c r="I78">
-        <v>423</v>
-      </c>
-      <c r="J78">
-        <v>524</v>
-      </c>
-      <c r="K78">
-        <v>608</v>
-      </c>
-      <c r="L78">
-        <v>692</v>
-      </c>
-      <c r="M78">
-        <v>776</v>
-      </c>
-      <c r="N78" s="14">
-        <v>861</v>
-      </c>
-      <c r="O78">
-        <v>72</v>
-      </c>
-      <c r="P78">
-        <v>105</v>
-      </c>
-      <c r="Q78">
-        <v>140</v>
-      </c>
-      <c r="R78">
-        <v>188</v>
-      </c>
-      <c r="S78" s="14">
-        <v>240</v>
-      </c>
-      <c r="T78">
-        <v>337</v>
-      </c>
-      <c r="U78">
-        <v>445</v>
-      </c>
-      <c r="V78">
-        <v>567</v>
-      </c>
-      <c r="W78">
-        <v>683</v>
-      </c>
-      <c r="X78">
-        <v>792</v>
-      </c>
-      <c r="Y78">
-        <v>901</v>
-      </c>
-      <c r="Z78">
-        <v>1010</v>
-      </c>
-      <c r="AA78">
-        <v>1119</v>
-      </c>
+      <c r="A78" s="44">
+        <v>76</v>
+      </c>
+      <c r="N78" s="14"/>
+      <c r="S78" s="14"/>
       <c r="AI78" s="14"/>
       <c r="AJ78">
-        <v>56</v>
+        <v>70</v>
       </c>
       <c r="AK78">
-        <v>73</v>
+        <v>94</v>
       </c>
       <c r="AL78">
-        <v>91</v>
+        <v>118</v>
       </c>
       <c r="AM78">
-        <v>121</v>
+        <v>159</v>
       </c>
       <c r="AN78" s="14">
-        <v>155</v>
+        <v>205</v>
       </c>
       <c r="AO78">
-        <v>204</v>
+        <v>272</v>
       </c>
       <c r="AP78">
-        <v>293</v>
+        <v>392</v>
       </c>
       <c r="AQ78">
-        <v>360</v>
+        <v>484</v>
       </c>
       <c r="AR78">
+        <v>104</v>
+      </c>
+      <c r="AS78">
+        <v>147</v>
+      </c>
+      <c r="AT78" s="16">
+        <v>194</v>
+      </c>
+      <c r="AU78">
+        <v>283</v>
+      </c>
+      <c r="AV78" s="14">
+        <v>368</v>
+      </c>
+      <c r="AW78">
+        <v>532</v>
+      </c>
+      <c r="AX78">
+        <v>698</v>
+      </c>
+      <c r="AY78">
+        <v>865</v>
+      </c>
+    </row>
+    <row r="79" spans="1:51" x14ac:dyDescent="0.35">
+      <c r="A79" s="44">
         <v>77</v>
-      </c>
-      <c r="AS78">
-        <v>107</v>
-      </c>
-      <c r="AT78" s="16">
-        <v>140</v>
-      </c>
-      <c r="AU78">
-        <v>202</v>
-      </c>
-      <c r="AV78" s="14">
-        <v>261</v>
-      </c>
-      <c r="AW78">
-        <v>376</v>
-      </c>
-      <c r="AX78">
-        <v>492</v>
-      </c>
-      <c r="AY78">
-        <v>609</v>
-      </c>
-    </row>
-    <row r="79" spans="1:51" x14ac:dyDescent="0.35">
-      <c r="A79" s="21">
-        <v>76</v>
       </c>
       <c r="N79" s="14"/>
       <c r="S79" s="14"/>
@@ -18342,8 +18220,8 @@
       </c>
     </row>
     <row r="80" spans="1:51" x14ac:dyDescent="0.35">
-      <c r="A80" s="21">
-        <v>77</v>
+      <c r="A80" s="44">
+        <v>78</v>
       </c>
       <c r="N80" s="14"/>
       <c r="S80" s="14"/>
@@ -18398,8 +18276,8 @@
       </c>
     </row>
     <row r="81" spans="1:51" x14ac:dyDescent="0.35">
-      <c r="A81" s="21">
-        <v>78</v>
+      <c r="A81" s="44">
+        <v>79</v>
       </c>
       <c r="N81" s="14"/>
       <c r="S81" s="14"/>
@@ -18454,8 +18332,8 @@
       </c>
     </row>
     <row r="82" spans="1:51" x14ac:dyDescent="0.35">
-      <c r="A82" s="21">
-        <v>79</v>
+      <c r="A82" s="44">
+        <v>80</v>
       </c>
       <c r="N82" s="14"/>
       <c r="S82" s="14"/>
@@ -18510,64 +18388,64 @@
       </c>
     </row>
     <row r="83" spans="1:51" x14ac:dyDescent="0.35">
-      <c r="A83" s="21">
-        <v>80</v>
+      <c r="A83" s="44">
+        <v>81</v>
       </c>
       <c r="N83" s="14"/>
       <c r="S83" s="14"/>
       <c r="AI83" s="14"/>
       <c r="AJ83">
-        <v>70</v>
+        <v>90</v>
       </c>
       <c r="AK83">
-        <v>94</v>
+        <v>123</v>
       </c>
       <c r="AL83">
-        <v>118</v>
+        <v>156</v>
       </c>
       <c r="AM83">
-        <v>159</v>
+        <v>212</v>
       </c>
       <c r="AN83" s="14">
-        <v>205</v>
+        <v>274</v>
       </c>
       <c r="AO83">
-        <v>272</v>
+        <v>367</v>
       </c>
       <c r="AP83">
-        <v>392</v>
+        <v>530</v>
       </c>
       <c r="AQ83">
-        <v>484</v>
+        <v>656</v>
       </c>
       <c r="AR83">
-        <v>104</v>
+        <v>143</v>
       </c>
       <c r="AS83">
-        <v>147</v>
+        <v>203</v>
       </c>
       <c r="AT83" s="16">
-        <v>194</v>
+        <v>269</v>
       </c>
       <c r="AU83">
-        <v>283</v>
+        <v>395</v>
       </c>
       <c r="AV83" s="14">
-        <v>368</v>
+        <v>516</v>
       </c>
       <c r="AW83">
-        <v>532</v>
+        <v>749</v>
       </c>
       <c r="AX83">
-        <v>698</v>
+        <v>985</v>
       </c>
       <c r="AY83">
-        <v>865</v>
+        <v>1221</v>
       </c>
     </row>
     <row r="84" spans="1:51" x14ac:dyDescent="0.35">
-      <c r="A84" s="21">
-        <v>81</v>
+      <c r="A84" s="44">
+        <v>82</v>
       </c>
       <c r="N84" s="14"/>
       <c r="S84" s="14"/>
@@ -18622,8 +18500,8 @@
       </c>
     </row>
     <row r="85" spans="1:51" x14ac:dyDescent="0.35">
-      <c r="A85" s="21">
-        <v>82</v>
+      <c r="A85" s="44">
+        <v>83</v>
       </c>
       <c r="N85" s="14"/>
       <c r="S85" s="14"/>
@@ -18678,8 +18556,8 @@
       </c>
     </row>
     <row r="86" spans="1:51" x14ac:dyDescent="0.35">
-      <c r="A86" s="21">
-        <v>83</v>
+      <c r="A86" s="44">
+        <v>84</v>
       </c>
       <c r="N86" s="14"/>
       <c r="S86" s="14"/>
@@ -18734,8 +18612,8 @@
       </c>
     </row>
     <row r="87" spans="1:51" x14ac:dyDescent="0.35">
-      <c r="A87" s="21">
-        <v>84</v>
+      <c r="A87" s="44">
+        <v>85</v>
       </c>
       <c r="N87" s="14"/>
       <c r="S87" s="14"/>
@@ -18789,64 +18667,9 @@
         <v>1221</v>
       </c>
     </row>
-    <row r="88" spans="1:51" x14ac:dyDescent="0.35">
-      <c r="A88" s="21">
-        <v>85</v>
-      </c>
-      <c r="N88" s="14"/>
-      <c r="S88" s="14"/>
-      <c r="AI88" s="14"/>
-      <c r="AJ88">
-        <v>90</v>
-      </c>
-      <c r="AK88">
-        <v>123</v>
-      </c>
-      <c r="AL88">
-        <v>156</v>
-      </c>
-      <c r="AM88">
-        <v>212</v>
-      </c>
-      <c r="AN88" s="14">
-        <v>274</v>
-      </c>
-      <c r="AO88">
-        <v>367</v>
-      </c>
-      <c r="AP88">
-        <v>530</v>
-      </c>
-      <c r="AQ88">
-        <v>656</v>
-      </c>
-      <c r="AR88">
-        <v>143</v>
-      </c>
-      <c r="AS88">
-        <v>203</v>
-      </c>
-      <c r="AT88" s="16">
-        <v>269</v>
-      </c>
-      <c r="AU88">
-        <v>395</v>
-      </c>
-      <c r="AV88" s="14">
-        <v>516</v>
-      </c>
-      <c r="AW88">
-        <v>749</v>
-      </c>
-      <c r="AX88">
-        <v>985</v>
-      </c>
-      <c r="AY88">
-        <v>1221</v>
-      </c>
-    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
 
@@ -18860,64 +18683,64 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="7" max="7" width="12.08984375" customWidth="1"/>
+    <col min="7" max="7" width="12.08984375" customWidth="1" collapsed="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:9" x14ac:dyDescent="0.35">
-      <c r="A1" s="40" t="s">
+      <c r="A1" s="32" t="s">
         <v>13</v>
       </c>
-      <c r="B1" s="40" t="s">
+      <c r="B1" s="32" t="s">
         <v>150</v>
       </c>
-      <c r="C1" s="40" t="s">
+      <c r="C1" s="32" t="s">
         <v>11</v>
       </c>
-      <c r="D1" s="40" t="s">
+      <c r="D1" s="32" t="s">
         <v>151</v>
       </c>
-      <c r="E1" s="40" t="s">
+      <c r="E1" s="32" t="s">
         <v>157</v>
       </c>
-      <c r="F1" s="40" t="s">
+      <c r="F1" s="32" t="s">
         <v>15</v>
       </c>
-      <c r="G1" s="40" t="s">
+      <c r="G1" s="32" t="s">
         <v>152</v>
       </c>
-      <c r="H1" s="40" t="s">
+      <c r="H1" s="32" t="s">
         <v>153</v>
       </c>
-      <c r="I1" s="40" t="s">
+      <c r="I1" s="32" t="s">
         <v>154</v>
       </c>
     </row>
     <row r="2" spans="1:9" x14ac:dyDescent="0.35">
-      <c r="A2" s="40" t="s">
+      <c r="A2" s="32" t="s">
         <v>18</v>
       </c>
-      <c r="B2" s="40" t="s">
+      <c r="B2" s="32" t="s">
         <v>172</v>
       </c>
-      <c r="C2" s="40" t="s">
+      <c r="C2" s="32" t="s">
         <v>169</v>
       </c>
-      <c r="D2" s="40" t="s">
+      <c r="D2" s="32" t="s">
         <v>173</v>
       </c>
-      <c r="E2" s="43" t="s">
+      <c r="E2" s="35" t="s">
         <v>171</v>
       </c>
-      <c r="F2" s="40" t="s">
+      <c r="F2" s="32" t="s">
         <v>17</v>
       </c>
-      <c r="G2" s="42" t="s">
+      <c r="G2" s="34" t="s">
         <v>170</v>
       </c>
-      <c r="H2" s="40" t="s">
+      <c r="H2" s="32" t="s">
         <v>156</v>
       </c>
-      <c r="I2" s="41">
+      <c r="I2" s="33">
         <v>44562</v>
       </c>
     </row>
@@ -18939,65 +18762,65 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="11.81640625" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="12.08984375" customWidth="1"/>
+    <col min="1" max="1" width="11.81640625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="7" max="7" width="12.08984375" customWidth="1" collapsed="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:9" x14ac:dyDescent="0.35">
-      <c r="A1" s="40" t="s">
+      <c r="A1" s="32" t="s">
         <v>13</v>
       </c>
-      <c r="B1" s="40" t="s">
+      <c r="B1" s="32" t="s">
         <v>150</v>
       </c>
-      <c r="C1" s="40" t="s">
+      <c r="C1" s="32" t="s">
         <v>11</v>
       </c>
-      <c r="D1" s="40" t="s">
+      <c r="D1" s="32" t="s">
         <v>151</v>
       </c>
-      <c r="E1" s="40" t="s">
+      <c r="E1" s="32" t="s">
         <v>14</v>
       </c>
-      <c r="F1" s="40" t="s">
+      <c r="F1" s="32" t="s">
         <v>15</v>
       </c>
-      <c r="G1" s="40" t="s">
+      <c r="G1" s="32" t="s">
         <v>152</v>
       </c>
-      <c r="H1" s="40" t="s">
+      <c r="H1" s="32" t="s">
         <v>153</v>
       </c>
-      <c r="I1" s="40" t="s">
+      <c r="I1" s="32" t="s">
         <v>154</v>
       </c>
     </row>
     <row r="2" spans="1:9" x14ac:dyDescent="0.35">
-      <c r="A2" s="40" t="s">
+      <c r="A2" s="32" t="s">
         <v>18</v>
       </c>
-      <c r="B2" s="40" t="s">
+      <c r="B2" s="32" t="s">
         <v>164</v>
       </c>
-      <c r="C2" s="40" t="s">
+      <c r="C2" s="32" t="s">
         <v>155</v>
       </c>
-      <c r="D2" s="40" t="s">
+      <c r="D2" s="32" t="s">
         <v>165</v>
       </c>
-      <c r="E2" s="43" t="s">
+      <c r="E2" s="35" t="s">
         <v>167</v>
       </c>
-      <c r="F2" s="40" t="s">
+      <c r="F2" s="32" t="s">
         <v>17</v>
       </c>
-      <c r="G2" s="42" t="s">
+      <c r="G2" s="34" t="s">
         <v>174</v>
       </c>
-      <c r="H2" s="40" t="s">
+      <c r="H2" s="32" t="s">
         <v>156</v>
       </c>
-      <c r="I2" s="43" t="s">
+      <c r="I2" s="35" t="s">
         <v>168</v>
       </c>
     </row>

</xml_diff>